<commit_message>
updates for compatibility with cvasi 1.5.0
</commit_message>
<xml_diff>
--- a/data-raw/parameter_descriptions.xlsx
+++ b/data-raw/parameter_descriptions.xlsx
@@ -1,26 +1,39 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27928"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29029"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\dev\cvasi-ui\inst\extdata\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\dev\cvasi-ui\data-raw\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4DF86F17-ECA4-43A3-A837-E6DD20587BA2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5E0BFB23-5272-4092-BD5F-E4F35DA3BBD0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16776" xr2:uid="{DB06E07F-B092-407E-AC5D-7A41EA44CF6C}"/>
   </bookViews>
   <sheets>
     <sheet name="parameter_descriptions4" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="863" uniqueCount="229">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="947" uniqueCount="227">
   <si>
     <t>model</t>
   </si>
@@ -163,15 +176,6 @@
     <t>Slope of concentration effect curve at EC_50</t>
   </si>
   <si>
-    <t>k</t>
-  </si>
-  <si>
-    <t>Degradation rate of toxicant in aquatic environments</t>
-  </si>
-  <si>
-    <t>degradation</t>
-  </si>
-  <si>
     <t>A</t>
   </si>
   <si>
@@ -193,24 +197,12 @@
     <t>Mass of phosphorous external</t>
   </si>
   <si>
-    <t>C</t>
-  </si>
-  <si>
-    <t>external substance concentration</t>
-  </si>
-  <si>
-    <t>Myriophyllum</t>
-  </si>
-  <si>
     <t>k_photo_max</t>
   </si>
   <si>
     <t>Maximum photosynthesis rate</t>
   </si>
   <si>
-    <t>lower default value than for Lemna, because  Myriophyllum grows slower than Lemna</t>
-  </si>
-  <si>
     <t>EC50_int</t>
   </si>
   <si>
@@ -707,6 +699,21 @@
   </si>
   <si>
     <t>µg fresh wt/mL</t>
+  </si>
+  <si>
+    <t>mu_control</t>
+  </si>
+  <si>
+    <t>lower default value than for Lemna, because macrophytes grow slower than Lemna</t>
+  </si>
+  <si>
+    <t>Magma-exp</t>
+  </si>
+  <si>
+    <t>Magma-log</t>
+  </si>
+  <si>
+    <t>D_L</t>
   </si>
 </sst>
 </file>
@@ -1568,13 +1575,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{09BDBC4E-EAE3-4956-99A4-F01BA4493ED9}">
-  <dimension ref="A1:K122"/>
+  <dimension ref="A1:K134"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M15" sqref="M15"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="B46" sqref="B46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="28.44140625" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
@@ -1680,7 +1690,7 @@
         <v>21</v>
       </c>
       <c r="D4" t="s">
-        <v>207</v>
+        <v>200</v>
       </c>
       <c r="E4" t="s">
         <v>15</v>
@@ -1698,7 +1708,7 @@
         <v>10</v>
       </c>
       <c r="K4" t="s">
-        <v>208</v>
+        <v>201</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.3">
@@ -1741,7 +1751,7 @@
         <v>26</v>
       </c>
       <c r="D6" t="s">
-        <v>209</v>
+        <v>202</v>
       </c>
       <c r="E6" t="s">
         <v>15</v>
@@ -1759,7 +1769,7 @@
         <v>1</v>
       </c>
       <c r="K6" t="s">
-        <v>210</v>
+        <v>203</v>
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.3">
@@ -1773,7 +1783,7 @@
         <v>28</v>
       </c>
       <c r="D7" t="s">
-        <v>209</v>
+        <v>202</v>
       </c>
       <c r="E7" t="s">
         <v>15</v>
@@ -1791,7 +1801,7 @@
         <v>1</v>
       </c>
       <c r="K7" t="s">
-        <v>210</v>
+        <v>203</v>
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.3">
@@ -1863,7 +1873,7 @@
         <v>34</v>
       </c>
       <c r="D10" t="s">
-        <v>211</v>
+        <v>204</v>
       </c>
       <c r="E10" t="s">
         <v>15</v>
@@ -1892,7 +1902,7 @@
         <v>36</v>
       </c>
       <c r="D11" t="s">
-        <v>211</v>
+        <v>204</v>
       </c>
       <c r="E11" t="s">
         <v>15</v>
@@ -1921,7 +1931,7 @@
         <v>38</v>
       </c>
       <c r="D12" t="s">
-        <v>211</v>
+        <v>204</v>
       </c>
       <c r="E12" t="s">
         <v>15</v>
@@ -1950,7 +1960,7 @@
         <v>40</v>
       </c>
       <c r="D13" t="s">
-        <v>212</v>
+        <v>205</v>
       </c>
       <c r="E13" t="s">
         <v>15</v>
@@ -1979,7 +1989,7 @@
         <v>42</v>
       </c>
       <c r="D14" t="s">
-        <v>213</v>
+        <v>206</v>
       </c>
       <c r="E14" t="s">
         <v>43</v>
@@ -2037,7 +2047,7 @@
         <v>48</v>
       </c>
       <c r="D16" t="s">
-        <v>14</v>
+        <v>207</v>
       </c>
       <c r="E16" t="s">
         <v>49</v>
@@ -2051,8 +2061,11 @@
       <c r="H16">
         <v>0</v>
       </c>
-      <c r="I16">
-        <v>100</v>
+      <c r="I16" t="s">
+        <v>44</v>
+      </c>
+      <c r="K16" t="s">
+        <v>208</v>
       </c>
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.3">
@@ -2066,10 +2079,10 @@
         <v>51</v>
       </c>
       <c r="D17" t="s">
-        <v>214</v>
+        <v>209</v>
       </c>
       <c r="E17" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="F17" t="s">
         <v>16</v>
@@ -2080,11 +2093,11 @@
       <c r="H17">
         <v>0</v>
       </c>
-      <c r="I17" t="s">
-        <v>44</v>
+      <c r="I17" s="1">
+        <v>1E-3</v>
       </c>
       <c r="K17" t="s">
-        <v>215</v>
+        <v>203</v>
       </c>
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.3">
@@ -2092,16 +2105,16 @@
         <v>11</v>
       </c>
       <c r="B18" t="s">
+        <v>52</v>
+      </c>
+      <c r="C18" t="s">
         <v>53</v>
       </c>
-      <c r="C18" t="s">
-        <v>54</v>
-      </c>
       <c r="D18" t="s">
-        <v>216</v>
+        <v>209</v>
       </c>
       <c r="E18" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="F18" t="s">
         <v>16</v>
@@ -2112,60 +2125,60 @@
       <c r="H18">
         <v>0</v>
       </c>
-      <c r="I18" s="1">
-        <v>1E-3</v>
+      <c r="I18">
+        <v>50</v>
       </c>
       <c r="K18" t="s">
-        <v>210</v>
+        <v>203</v>
       </c>
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>11</v>
+        <v>224</v>
       </c>
       <c r="B19" t="s">
+        <v>222</v>
+      </c>
+      <c r="C19" t="s">
         <v>55</v>
       </c>
-      <c r="C19" t="s">
-        <v>56</v>
-      </c>
       <c r="D19" t="s">
-        <v>216</v>
+        <v>14</v>
       </c>
       <c r="E19" t="s">
-        <v>52</v>
+        <v>15</v>
       </c>
       <c r="F19" t="s">
         <v>16</v>
       </c>
-      <c r="G19" t="s">
-        <v>17</v>
+      <c r="G19">
+        <v>0.42</v>
       </c>
       <c r="H19">
         <v>0</v>
       </c>
       <c r="I19">
-        <v>50</v>
+        <v>1</v>
       </c>
       <c r="K19" t="s">
-        <v>210</v>
+        <v>223</v>
       </c>
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>11</v>
+        <v>224</v>
       </c>
       <c r="B20" t="s">
+        <v>56</v>
+      </c>
+      <c r="C20" t="s">
         <v>57</v>
       </c>
-      <c r="C20" t="s">
-        <v>58</v>
-      </c>
       <c r="D20" t="s">
-        <v>217</v>
+        <v>210</v>
       </c>
       <c r="E20" t="s">
-        <v>52</v>
+        <v>43</v>
       </c>
       <c r="F20" t="s">
         <v>16</v>
@@ -2182,25 +2195,25 @@
     </row>
     <row r="21" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
+        <v>224</v>
+      </c>
+      <c r="B21" t="s">
+        <v>58</v>
+      </c>
+      <c r="C21" t="s">
         <v>59</v>
       </c>
-      <c r="B21" t="s">
-        <v>60</v>
-      </c>
-      <c r="C21" t="s">
-        <v>61</v>
-      </c>
       <c r="D21" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="E21" t="s">
-        <v>15</v>
+        <v>43</v>
       </c>
       <c r="F21" t="s">
-        <v>16</v>
+        <v>60</v>
       </c>
       <c r="G21">
-        <v>0.42</v>
+        <v>1</v>
       </c>
       <c r="H21">
         <v>0</v>
@@ -2208,22 +2221,19 @@
       <c r="I21">
         <v>1</v>
       </c>
-      <c r="K21" t="s">
-        <v>62</v>
-      </c>
     </row>
     <row r="22" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
-        <v>59</v>
+        <v>224</v>
       </c>
       <c r="B22" t="s">
-        <v>63</v>
+        <v>45</v>
       </c>
       <c r="C22" t="s">
-        <v>64</v>
+        <v>46</v>
       </c>
       <c r="D22" t="s">
-        <v>217</v>
+        <v>17</v>
       </c>
       <c r="E22" t="s">
         <v>43</v>
@@ -2235,210 +2245,213 @@
         <v>17</v>
       </c>
       <c r="H22">
-        <v>0</v>
-      </c>
-      <c r="I22" t="s">
-        <v>44</v>
+        <v>0.1</v>
+      </c>
+      <c r="I22">
+        <v>20</v>
       </c>
     </row>
     <row r="23" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
-        <v>59</v>
+        <v>224</v>
       </c>
       <c r="B23" t="s">
-        <v>65</v>
+        <v>52</v>
       </c>
       <c r="C23" t="s">
-        <v>66</v>
+        <v>61</v>
       </c>
       <c r="D23" t="s">
-        <v>17</v>
+        <v>62</v>
       </c>
       <c r="E23" t="s">
-        <v>43</v>
+        <v>63</v>
       </c>
       <c r="F23" t="s">
-        <v>67</v>
-      </c>
-      <c r="G23">
-        <v>1</v>
+        <v>16</v>
+      </c>
+      <c r="G23" t="s">
+        <v>17</v>
       </c>
       <c r="H23">
         <v>0</v>
       </c>
       <c r="I23">
-        <v>1</v>
+        <v>100</v>
+      </c>
+      <c r="K23" t="s">
+        <v>64</v>
       </c>
     </row>
     <row r="24" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
-        <v>59</v>
+        <v>224</v>
       </c>
       <c r="B24" t="s">
-        <v>45</v>
+        <v>65</v>
       </c>
       <c r="C24" t="s">
-        <v>46</v>
+        <v>66</v>
       </c>
       <c r="D24" t="s">
-        <v>17</v>
+        <v>211</v>
       </c>
       <c r="E24" t="s">
-        <v>43</v>
+        <v>63</v>
       </c>
       <c r="F24" t="s">
-        <v>16</v>
-      </c>
-      <c r="G24" t="s">
-        <v>17</v>
+        <v>60</v>
+      </c>
+      <c r="G24">
+        <v>1000</v>
       </c>
       <c r="H24">
-        <v>0.1</v>
+        <v>10</v>
       </c>
       <c r="I24">
-        <v>20</v>
+        <v>100000</v>
       </c>
     </row>
     <row r="25" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
-        <v>59</v>
+        <v>224</v>
       </c>
       <c r="B25" t="s">
-        <v>55</v>
+        <v>67</v>
       </c>
       <c r="C25" t="s">
         <v>68</v>
       </c>
       <c r="D25" t="s">
-        <v>69</v>
+        <v>17</v>
       </c>
       <c r="E25" t="s">
-        <v>70</v>
+        <v>63</v>
       </c>
       <c r="F25" t="s">
-        <v>16</v>
-      </c>
-      <c r="G25" t="s">
-        <v>17</v>
+        <v>60</v>
+      </c>
+      <c r="G25">
+        <v>16.7</v>
       </c>
       <c r="H25">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I25">
-        <v>100</v>
-      </c>
-      <c r="K25" t="s">
-        <v>71</v>
+        <v>1000</v>
       </c>
     </row>
     <row r="26" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
-        <v>59</v>
+        <v>224</v>
       </c>
       <c r="B26" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="C26" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="D26" t="s">
-        <v>218</v>
+        <v>212</v>
       </c>
       <c r="E26" t="s">
-        <v>70</v>
+        <v>63</v>
       </c>
       <c r="F26" t="s">
-        <v>67</v>
+        <v>60</v>
       </c>
       <c r="G26">
-        <v>1000</v>
+        <v>1</v>
       </c>
       <c r="H26">
-        <v>10</v>
+        <v>0.5</v>
       </c>
       <c r="I26">
-        <v>100000</v>
+        <v>2</v>
       </c>
     </row>
     <row r="27" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
-        <v>59</v>
+        <v>224</v>
       </c>
       <c r="B27" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="C27" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="D27" t="s">
         <v>17</v>
       </c>
       <c r="E27" t="s">
-        <v>70</v>
+        <v>63</v>
       </c>
       <c r="F27" t="s">
-        <v>67</v>
-      </c>
-      <c r="G27">
-        <v>16.7</v>
+        <v>60</v>
+      </c>
+      <c r="G27" t="s">
+        <v>17</v>
       </c>
       <c r="H27">
-        <v>1</v>
-      </c>
-      <c r="I27">
-        <v>1000</v>
+        <v>0</v>
+      </c>
+      <c r="I27" t="s">
+        <v>44</v>
+      </c>
+      <c r="K27" t="s">
+        <v>73</v>
       </c>
     </row>
     <row r="28" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
-        <v>59</v>
+        <v>224</v>
       </c>
       <c r="B28" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="C28" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="D28" t="s">
-        <v>219</v>
+        <v>17</v>
       </c>
       <c r="E28" t="s">
-        <v>70</v>
+        <v>63</v>
       </c>
       <c r="F28" t="s">
-        <v>67</v>
+        <v>60</v>
       </c>
       <c r="G28">
         <v>1</v>
       </c>
       <c r="H28">
-        <v>0.5</v>
+        <v>0</v>
       </c>
       <c r="I28">
-        <v>2</v>
+        <v>100000</v>
       </c>
     </row>
     <row r="29" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
-        <v>59</v>
+        <v>224</v>
       </c>
       <c r="B29" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="C29" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="D29" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="E29" t="s">
-        <v>70</v>
+        <v>63</v>
       </c>
       <c r="F29" t="s">
-        <v>67</v>
-      </c>
-      <c r="G29" t="s">
-        <v>17</v>
+        <v>60</v>
+      </c>
+      <c r="G29">
+        <v>0</v>
       </c>
       <c r="H29">
         <v>0</v>
@@ -2446,60 +2459,57 @@
       <c r="I29" t="s">
         <v>44</v>
       </c>
-      <c r="K29" t="s">
-        <v>80</v>
-      </c>
     </row>
     <row r="30" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
-        <v>59</v>
+        <v>224</v>
       </c>
       <c r="B30" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="C30" t="s">
-        <v>82</v>
+        <v>48</v>
       </c>
       <c r="D30" t="s">
-        <v>17</v>
+        <v>213</v>
       </c>
       <c r="E30" t="s">
-        <v>70</v>
+        <v>49</v>
       </c>
       <c r="F30" t="s">
-        <v>67</v>
-      </c>
-      <c r="G30">
-        <v>1</v>
+        <v>16</v>
+      </c>
+      <c r="G30" t="s">
+        <v>17</v>
       </c>
       <c r="H30">
         <v>0</v>
       </c>
-      <c r="I30">
-        <v>100000</v>
+      <c r="I30" t="s">
+        <v>44</v>
       </c>
     </row>
     <row r="31" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
-        <v>59</v>
+        <v>224</v>
       </c>
       <c r="B31" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="C31" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="D31" t="s">
-        <v>14</v>
+        <v>214</v>
       </c>
       <c r="E31" t="s">
-        <v>70</v>
+        <v>49</v>
       </c>
       <c r="F31" t="s">
-        <v>67</v>
-      </c>
-      <c r="G31">
-        <v>0</v>
+        <v>16</v>
+      </c>
+      <c r="G31" t="s">
+        <v>17</v>
       </c>
       <c r="H31">
         <v>0</v>
@@ -2510,48 +2520,51 @@
     </row>
     <row r="32" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
-        <v>59</v>
+        <v>225</v>
       </c>
       <c r="B32" t="s">
-        <v>85</v>
+        <v>222</v>
       </c>
       <c r="C32" t="s">
-        <v>51</v>
+        <v>55</v>
       </c>
       <c r="D32" t="s">
-        <v>220</v>
+        <v>14</v>
       </c>
       <c r="E32" t="s">
-        <v>52</v>
+        <v>15</v>
       </c>
       <c r="F32" t="s">
         <v>16</v>
       </c>
-      <c r="G32" t="s">
-        <v>17</v>
+      <c r="G32">
+        <v>0.42</v>
       </c>
       <c r="H32">
         <v>0</v>
       </c>
-      <c r="I32" t="s">
-        <v>44</v>
+      <c r="I32">
+        <v>1</v>
+      </c>
+      <c r="K32" t="s">
+        <v>223</v>
       </c>
     </row>
     <row r="33" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
-        <v>59</v>
+        <v>225</v>
       </c>
       <c r="B33" t="s">
-        <v>86</v>
+        <v>56</v>
       </c>
       <c r="C33" t="s">
-        <v>87</v>
+        <v>57</v>
       </c>
       <c r="D33" t="s">
-        <v>221</v>
+        <v>210</v>
       </c>
       <c r="E33" t="s">
-        <v>52</v>
+        <v>43</v>
       </c>
       <c r="F33" t="s">
         <v>16</v>
@@ -2568,83 +2581,77 @@
     </row>
     <row r="34" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
+        <v>225</v>
+      </c>
+      <c r="B34" t="s">
+        <v>58</v>
+      </c>
+      <c r="C34" t="s">
         <v>59</v>
       </c>
-      <c r="B34" t="s">
-        <v>88</v>
-      </c>
-      <c r="C34" t="s">
-        <v>89</v>
-      </c>
       <c r="D34" t="s">
-        <v>220</v>
+        <v>17</v>
       </c>
       <c r="E34" t="s">
-        <v>15</v>
+        <v>43</v>
       </c>
       <c r="F34" t="s">
-        <v>16</v>
-      </c>
-      <c r="G34" t="s">
-        <v>17</v>
+        <v>60</v>
+      </c>
+      <c r="G34">
+        <v>1</v>
       </c>
       <c r="H34">
         <v>0</v>
       </c>
-      <c r="I34" t="s">
-        <v>44</v>
+      <c r="I34">
+        <v>1</v>
       </c>
     </row>
     <row r="35" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
-        <v>90</v>
+        <v>225</v>
       </c>
       <c r="B35" t="s">
-        <v>91</v>
+        <v>45</v>
       </c>
       <c r="C35" t="s">
-        <v>92</v>
+        <v>46</v>
       </c>
       <c r="D35" t="s">
-        <v>93</v>
+        <v>17</v>
       </c>
       <c r="E35" t="s">
-        <v>15</v>
+        <v>43</v>
       </c>
       <c r="F35" t="s">
-        <v>67</v>
-      </c>
-      <c r="G35" t="b">
-        <v>1</v>
+        <v>16</v>
+      </c>
+      <c r="G35" t="s">
+        <v>17</v>
       </c>
       <c r="H35">
-        <v>0</v>
+        <v>0.1</v>
       </c>
       <c r="I35">
-        <v>1</v>
-      </c>
-      <c r="J35" t="s">
-        <v>94</v>
-      </c>
-      <c r="K35" t="s">
-        <v>95</v>
+        <v>20</v>
       </c>
     </row>
     <row r="36" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
-        <v>90</v>
+        <v>225</v>
       </c>
       <c r="B36" t="s">
-        <v>96</v>
+        <v>52</v>
       </c>
       <c r="C36" t="s">
         <v>61</v>
       </c>
       <c r="D36" t="s">
-        <v>14</v>
+        <v>62</v>
       </c>
       <c r="E36" t="s">
-        <v>15</v>
+        <v>63</v>
       </c>
       <c r="F36" t="s">
         <v>16</v>
@@ -2656,201 +2663,207 @@
         <v>0</v>
       </c>
       <c r="I36">
-        <v>1</v>
+        <v>100</v>
+      </c>
+      <c r="K36" t="s">
+        <v>64</v>
       </c>
     </row>
     <row r="37" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
-        <v>90</v>
+        <v>225</v>
       </c>
       <c r="B37" t="s">
-        <v>97</v>
+        <v>65</v>
       </c>
       <c r="C37" t="s">
-        <v>98</v>
+        <v>66</v>
       </c>
       <c r="D37" t="s">
-        <v>14</v>
+        <v>211</v>
       </c>
       <c r="E37" t="s">
-        <v>15</v>
+        <v>63</v>
       </c>
       <c r="F37" t="s">
-        <v>67</v>
+        <v>60</v>
       </c>
       <c r="G37">
-        <v>0</v>
+        <v>1000</v>
       </c>
       <c r="H37">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="I37">
-        <v>0.3</v>
+        <v>100000</v>
       </c>
     </row>
     <row r="38" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
-        <v>90</v>
+        <v>225</v>
       </c>
       <c r="B38" t="s">
-        <v>99</v>
+        <v>67</v>
       </c>
       <c r="C38" t="s">
-        <v>100</v>
+        <v>68</v>
       </c>
       <c r="D38" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="E38" t="s">
-        <v>15</v>
+        <v>63</v>
       </c>
       <c r="F38" t="s">
-        <v>67</v>
-      </c>
-      <c r="G38" t="s">
-        <v>17</v>
+        <v>60</v>
+      </c>
+      <c r="G38">
+        <v>16.7</v>
       </c>
       <c r="H38">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I38">
-        <v>3</v>
+        <v>1000</v>
       </c>
     </row>
     <row r="39" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
-        <v>90</v>
+        <v>225</v>
       </c>
       <c r="B39" t="s">
-        <v>101</v>
+        <v>69</v>
       </c>
       <c r="C39" t="s">
-        <v>36</v>
+        <v>70</v>
       </c>
       <c r="D39" t="s">
-        <v>211</v>
+        <v>212</v>
       </c>
       <c r="E39" t="s">
-        <v>15</v>
+        <v>63</v>
       </c>
       <c r="F39" t="s">
-        <v>67</v>
-      </c>
-      <c r="G39" t="s">
-        <v>17</v>
+        <v>60</v>
+      </c>
+      <c r="G39">
+        <v>1</v>
       </c>
       <c r="H39">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="I39">
-        <v>40</v>
+        <v>2</v>
       </c>
     </row>
     <row r="40" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
-        <v>90</v>
+        <v>225</v>
       </c>
       <c r="B40" t="s">
-        <v>102</v>
+        <v>71</v>
       </c>
       <c r="C40" t="s">
-        <v>38</v>
+        <v>72</v>
       </c>
       <c r="D40" t="s">
-        <v>211</v>
+        <v>17</v>
       </c>
       <c r="E40" t="s">
-        <v>15</v>
+        <v>63</v>
       </c>
       <c r="F40" t="s">
-        <v>67</v>
+        <v>60</v>
       </c>
       <c r="G40" t="s">
         <v>17</v>
       </c>
       <c r="H40">
-        <v>4</v>
-      </c>
-      <c r="I40">
-        <v>50</v>
+        <v>0</v>
+      </c>
+      <c r="I40" t="s">
+        <v>44</v>
+      </c>
+      <c r="K40" t="s">
+        <v>73</v>
       </c>
     </row>
     <row r="41" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
-        <v>90</v>
+        <v>225</v>
       </c>
       <c r="B41" t="s">
-        <v>103</v>
+        <v>74</v>
       </c>
       <c r="C41" t="s">
-        <v>104</v>
+        <v>75</v>
       </c>
       <c r="D41" t="s">
-        <v>211</v>
+        <v>17</v>
       </c>
       <c r="E41" t="s">
-        <v>15</v>
+        <v>63</v>
       </c>
       <c r="F41" t="s">
-        <v>67</v>
-      </c>
-      <c r="G41" t="s">
-        <v>17</v>
+        <v>60</v>
+      </c>
+      <c r="G41">
+        <v>1</v>
       </c>
       <c r="H41">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="I41">
-        <v>40</v>
+        <v>100000</v>
       </c>
     </row>
     <row r="42" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
-        <v>90</v>
+        <v>225</v>
       </c>
       <c r="B42" t="s">
-        <v>105</v>
+        <v>76</v>
       </c>
       <c r="C42" t="s">
-        <v>106</v>
+        <v>77</v>
       </c>
       <c r="D42" t="s">
-        <v>211</v>
+        <v>14</v>
       </c>
       <c r="E42" t="s">
-        <v>15</v>
+        <v>63</v>
       </c>
       <c r="F42" t="s">
-        <v>67</v>
-      </c>
-      <c r="G42" t="s">
-        <v>17</v>
+        <v>60</v>
+      </c>
+      <c r="G42">
+        <v>0</v>
       </c>
       <c r="H42">
-        <v>4</v>
-      </c>
-      <c r="I42">
-        <v>40</v>
+        <v>0</v>
+      </c>
+      <c r="I42" t="s">
+        <v>44</v>
       </c>
     </row>
     <row r="43" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
-        <v>90</v>
+        <v>225</v>
       </c>
       <c r="B43" t="s">
-        <v>107</v>
+        <v>78</v>
       </c>
       <c r="C43" t="s">
-        <v>108</v>
+        <v>48</v>
       </c>
       <c r="D43" t="s">
-        <v>17</v>
+        <v>213</v>
       </c>
       <c r="E43" t="s">
-        <v>15</v>
+        <v>49</v>
       </c>
       <c r="F43" t="s">
-        <v>67</v>
+        <v>16</v>
       </c>
       <c r="G43" t="s">
         <v>17</v>
@@ -2858,28 +2871,28 @@
       <c r="H43">
         <v>0</v>
       </c>
-      <c r="I43">
-        <v>10</v>
+      <c r="I43" t="s">
+        <v>44</v>
       </c>
     </row>
     <row r="44" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
-        <v>90</v>
+        <v>225</v>
       </c>
       <c r="B44" t="s">
-        <v>109</v>
+        <v>79</v>
       </c>
       <c r="C44" t="s">
-        <v>110</v>
+        <v>80</v>
       </c>
       <c r="D44" t="s">
-        <v>14</v>
+        <v>214</v>
       </c>
       <c r="E44" t="s">
-        <v>15</v>
+        <v>49</v>
       </c>
       <c r="F44" t="s">
-        <v>67</v>
+        <v>16</v>
       </c>
       <c r="G44" t="s">
         <v>17</v>
@@ -2893,22 +2906,22 @@
     </row>
     <row r="45" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
-        <v>90</v>
+        <v>225</v>
       </c>
       <c r="B45" t="s">
-        <v>111</v>
+        <v>226</v>
       </c>
       <c r="C45" t="s">
-        <v>112</v>
+        <v>82</v>
       </c>
       <c r="D45" t="s">
-        <v>222</v>
+        <v>213</v>
       </c>
       <c r="E45" t="s">
         <v>15</v>
       </c>
       <c r="F45" t="s">
-        <v>67</v>
+        <v>16</v>
       </c>
       <c r="G45" t="s">
         <v>17</v>
@@ -2922,51 +2935,57 @@
     </row>
     <row r="46" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
-        <v>90</v>
+        <v>83</v>
       </c>
       <c r="B46" t="s">
-        <v>113</v>
+        <v>84</v>
       </c>
       <c r="C46" t="s">
-        <v>114</v>
+        <v>85</v>
       </c>
       <c r="D46" t="s">
-        <v>115</v>
+        <v>86</v>
       </c>
       <c r="E46" t="s">
         <v>15</v>
       </c>
       <c r="F46" t="s">
-        <v>67</v>
-      </c>
-      <c r="G46" t="s">
-        <v>17</v>
+        <v>60</v>
+      </c>
+      <c r="G46" t="b">
+        <v>1</v>
       </c>
       <c r="H46">
         <v>0</v>
       </c>
       <c r="I46">
-        <v>10</v>
+        <v>1</v>
+      </c>
+      <c r="J46" t="s">
+        <v>87</v>
+      </c>
+      <c r="K46" t="s">
+        <v>88</v>
       </c>
     </row>
     <row r="47" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
-        <v>90</v>
+        <v>83</v>
       </c>
       <c r="B47" t="s">
-        <v>116</v>
+        <v>89</v>
       </c>
       <c r="C47" t="s">
-        <v>117</v>
+        <v>55</v>
       </c>
       <c r="D47" t="s">
-        <v>115</v>
+        <v>14</v>
       </c>
       <c r="E47" t="s">
         <v>15</v>
       </c>
       <c r="F47" t="s">
-        <v>67</v>
+        <v>16</v>
       </c>
       <c r="G47" t="s">
         <v>17</v>
@@ -2975,88 +2994,85 @@
         <v>0</v>
       </c>
       <c r="I47">
-        <v>10</v>
-      </c>
-      <c r="K47" t="s">
-        <v>118</v>
+        <v>1</v>
       </c>
     </row>
     <row r="48" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
+        <v>83</v>
+      </c>
+      <c r="B48" t="s">
         <v>90</v>
       </c>
-      <c r="B48" t="s">
-        <v>119</v>
-      </c>
       <c r="C48" t="s">
-        <v>120</v>
+        <v>91</v>
       </c>
       <c r="D48" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="E48" t="s">
         <v>15</v>
       </c>
       <c r="F48" t="s">
-        <v>67</v>
-      </c>
-      <c r="G48" t="s">
-        <v>17</v>
+        <v>60</v>
+      </c>
+      <c r="G48">
+        <v>0</v>
       </c>
       <c r="H48">
         <v>0</v>
       </c>
       <c r="I48">
-        <v>20</v>
+        <v>0.3</v>
       </c>
     </row>
     <row r="49" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
-        <v>90</v>
+        <v>83</v>
       </c>
       <c r="B49" t="s">
-        <v>121</v>
+        <v>92</v>
       </c>
       <c r="C49" t="s">
-        <v>122</v>
+        <v>93</v>
       </c>
       <c r="D49" t="s">
-        <v>115</v>
+        <v>14</v>
       </c>
       <c r="E49" t="s">
         <v>15</v>
       </c>
       <c r="F49" t="s">
-        <v>67</v>
+        <v>60</v>
       </c>
       <c r="G49" t="s">
         <v>17</v>
       </c>
       <c r="H49">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I49">
-        <v>10000</v>
+        <v>3</v>
       </c>
     </row>
     <row r="50" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
-        <v>90</v>
+        <v>83</v>
       </c>
       <c r="B50" t="s">
-        <v>123</v>
+        <v>94</v>
       </c>
       <c r="C50" t="s">
-        <v>124</v>
+        <v>36</v>
       </c>
       <c r="D50" t="s">
-        <v>115</v>
+        <v>204</v>
       </c>
       <c r="E50" t="s">
         <v>15</v>
       </c>
       <c r="F50" t="s">
-        <v>67</v>
+        <v>60</v>
       </c>
       <c r="G50" t="s">
         <v>17</v>
@@ -3065,236 +3081,230 @@
         <v>0</v>
       </c>
       <c r="I50">
-        <v>10</v>
+        <v>40</v>
       </c>
     </row>
     <row r="51" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
-        <v>90</v>
+        <v>83</v>
       </c>
       <c r="B51" t="s">
-        <v>125</v>
+        <v>95</v>
       </c>
       <c r="C51" t="s">
-        <v>126</v>
+        <v>38</v>
       </c>
       <c r="D51" t="s">
-        <v>115</v>
+        <v>204</v>
       </c>
       <c r="E51" t="s">
         <v>15</v>
       </c>
       <c r="F51" t="s">
-        <v>67</v>
+        <v>60</v>
       </c>
       <c r="G51" t="s">
         <v>17</v>
       </c>
       <c r="H51">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="I51">
-        <v>10</v>
-      </c>
-      <c r="K51" t="s">
-        <v>127</v>
+        <v>50</v>
       </c>
     </row>
     <row r="52" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
-        <v>90</v>
+        <v>83</v>
       </c>
       <c r="B52" t="s">
-        <v>128</v>
+        <v>96</v>
       </c>
       <c r="C52" t="s">
-        <v>120</v>
+        <v>97</v>
       </c>
       <c r="D52" t="s">
-        <v>17</v>
+        <v>204</v>
       </c>
       <c r="E52" t="s">
         <v>15</v>
       </c>
       <c r="F52" t="s">
-        <v>67</v>
+        <v>60</v>
       </c>
       <c r="G52" t="s">
         <v>17</v>
       </c>
       <c r="H52">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="I52">
-        <v>20</v>
+        <v>40</v>
       </c>
     </row>
     <row r="53" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
-        <v>90</v>
+        <v>83</v>
       </c>
       <c r="B53" t="s">
-        <v>129</v>
+        <v>98</v>
       </c>
       <c r="C53" t="s">
-        <v>130</v>
+        <v>99</v>
       </c>
       <c r="D53" t="s">
-        <v>115</v>
+        <v>204</v>
       </c>
       <c r="E53" t="s">
         <v>15</v>
       </c>
       <c r="F53" t="s">
-        <v>67</v>
+        <v>60</v>
       </c>
       <c r="G53" t="s">
         <v>17</v>
       </c>
       <c r="H53">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="I53">
-        <v>10000</v>
+        <v>40</v>
       </c>
     </row>
     <row r="54" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
-        <v>90</v>
+        <v>83</v>
       </c>
       <c r="B54" t="s">
-        <v>131</v>
+        <v>100</v>
       </c>
       <c r="C54" t="s">
-        <v>132</v>
+        <v>101</v>
       </c>
       <c r="D54" t="s">
-        <v>223</v>
+        <v>17</v>
       </c>
       <c r="E54" t="s">
         <v>15</v>
       </c>
       <c r="F54" t="s">
-        <v>67</v>
+        <v>60</v>
       </c>
       <c r="G54" t="s">
         <v>17</v>
       </c>
       <c r="H54">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I54">
-        <v>10000</v>
+        <v>10</v>
       </c>
     </row>
     <row r="55" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
-        <v>90</v>
+        <v>83</v>
       </c>
       <c r="B55" t="s">
-        <v>133</v>
+        <v>102</v>
       </c>
       <c r="C55" t="s">
-        <v>134</v>
+        <v>103</v>
       </c>
       <c r="D55" t="s">
-        <v>135</v>
+        <v>14</v>
       </c>
       <c r="E55" t="s">
         <v>15</v>
       </c>
       <c r="F55" t="s">
-        <v>67</v>
+        <v>60</v>
       </c>
       <c r="G55" t="s">
         <v>17</v>
       </c>
-      <c r="H55" s="1">
-        <v>9.9999999999999995E-7</v>
-      </c>
-      <c r="I55" s="1">
-        <v>0.01</v>
-      </c>
-      <c r="K55" t="s">
-        <v>136</v>
+      <c r="H55">
+        <v>0</v>
+      </c>
+      <c r="I55" t="s">
+        <v>44</v>
       </c>
     </row>
     <row r="56" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A56" t="s">
-        <v>90</v>
+        <v>83</v>
       </c>
       <c r="B56" t="s">
-        <v>137</v>
+        <v>104</v>
       </c>
       <c r="C56" t="s">
-        <v>138</v>
+        <v>105</v>
       </c>
       <c r="D56" t="s">
-        <v>139</v>
+        <v>215</v>
       </c>
       <c r="E56" t="s">
         <v>15</v>
       </c>
       <c r="F56" t="s">
-        <v>67</v>
+        <v>60</v>
       </c>
       <c r="G56" t="s">
         <v>17</v>
       </c>
       <c r="H56">
-        <v>1</v>
-      </c>
-      <c r="I56">
-        <v>100</v>
+        <v>0</v>
+      </c>
+      <c r="I56" t="s">
+        <v>44</v>
       </c>
     </row>
     <row r="57" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A57" t="s">
-        <v>90</v>
+        <v>83</v>
       </c>
       <c r="B57" t="s">
-        <v>140</v>
+        <v>106</v>
       </c>
       <c r="C57" t="s">
-        <v>141</v>
+        <v>107</v>
       </c>
       <c r="D57" t="s">
-        <v>17</v>
+        <v>108</v>
       </c>
       <c r="E57" t="s">
-        <v>43</v>
+        <v>15</v>
       </c>
       <c r="F57" t="s">
-        <v>67</v>
-      </c>
-      <c r="G57">
-        <v>1</v>
+        <v>60</v>
+      </c>
+      <c r="G57" t="s">
+        <v>17</v>
       </c>
       <c r="H57">
         <v>0</v>
       </c>
       <c r="I57">
-        <v>1</v>
+        <v>10</v>
       </c>
     </row>
     <row r="58" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A58" t="s">
-        <v>90</v>
+        <v>83</v>
       </c>
       <c r="B58" t="s">
-        <v>142</v>
+        <v>109</v>
       </c>
       <c r="C58" t="s">
-        <v>42</v>
+        <v>110</v>
       </c>
       <c r="D58" t="s">
-        <v>217</v>
+        <v>108</v>
       </c>
       <c r="E58" t="s">
-        <v>43</v>
+        <v>15</v>
       </c>
       <c r="F58" t="s">
-        <v>16</v>
+        <v>60</v>
       </c>
       <c r="G58" t="s">
         <v>17</v>
@@ -3302,34 +3312,37 @@
       <c r="H58">
         <v>0</v>
       </c>
-      <c r="I58" t="s">
-        <v>44</v>
+      <c r="I58">
+        <v>10</v>
+      </c>
+      <c r="K58" t="s">
+        <v>111</v>
       </c>
     </row>
     <row r="59" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A59" t="s">
-        <v>90</v>
+        <v>83</v>
       </c>
       <c r="B59" t="s">
-        <v>45</v>
+        <v>112</v>
       </c>
       <c r="C59" t="s">
-        <v>46</v>
+        <v>113</v>
       </c>
       <c r="D59" t="s">
         <v>17</v>
       </c>
       <c r="E59" t="s">
-        <v>43</v>
+        <v>15</v>
       </c>
       <c r="F59" t="s">
-        <v>16</v>
+        <v>60</v>
       </c>
       <c r="G59" t="s">
         <v>17</v>
       </c>
       <c r="H59">
-        <v>0.1</v>
+        <v>0</v>
       </c>
       <c r="I59">
         <v>20</v>
@@ -3337,54 +3350,51 @@
     </row>
     <row r="60" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A60" t="s">
-        <v>90</v>
+        <v>83</v>
       </c>
       <c r="B60" t="s">
-        <v>143</v>
+        <v>114</v>
       </c>
       <c r="C60" t="s">
-        <v>144</v>
+        <v>115</v>
       </c>
       <c r="D60" t="s">
-        <v>69</v>
+        <v>108</v>
       </c>
       <c r="E60" t="s">
-        <v>70</v>
+        <v>15</v>
       </c>
       <c r="F60" t="s">
-        <v>16</v>
+        <v>60</v>
       </c>
       <c r="G60" t="s">
         <v>17</v>
       </c>
       <c r="H60">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I60">
-        <v>100</v>
-      </c>
-      <c r="K60" t="s">
-        <v>71</v>
+        <v>10000</v>
       </c>
     </row>
     <row r="61" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A61" t="s">
-        <v>90</v>
+        <v>83</v>
       </c>
       <c r="B61" t="s">
-        <v>145</v>
+        <v>116</v>
       </c>
       <c r="C61" t="s">
-        <v>146</v>
+        <v>117</v>
       </c>
       <c r="D61" t="s">
-        <v>224</v>
+        <v>108</v>
       </c>
       <c r="E61" t="s">
-        <v>70</v>
+        <v>15</v>
       </c>
       <c r="F61" t="s">
-        <v>67</v>
+        <v>60</v>
       </c>
       <c r="G61" t="s">
         <v>17</v>
@@ -3393,56 +3403,59 @@
         <v>0</v>
       </c>
       <c r="I61">
-        <v>100000</v>
+        <v>10</v>
       </c>
     </row>
     <row r="62" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A62" t="s">
-        <v>90</v>
+        <v>83</v>
       </c>
       <c r="B62" t="s">
-        <v>147</v>
+        <v>118</v>
       </c>
       <c r="C62" t="s">
-        <v>148</v>
+        <v>119</v>
       </c>
       <c r="D62" t="s">
-        <v>17</v>
+        <v>108</v>
       </c>
       <c r="E62" t="s">
-        <v>70</v>
+        <v>15</v>
       </c>
       <c r="F62" t="s">
-        <v>67</v>
-      </c>
-      <c r="G62">
-        <v>1</v>
+        <v>60</v>
+      </c>
+      <c r="G62" t="s">
+        <v>17</v>
       </c>
       <c r="H62">
         <v>0</v>
       </c>
       <c r="I62">
-        <v>100000</v>
+        <v>10</v>
+      </c>
+      <c r="K62" t="s">
+        <v>120</v>
       </c>
     </row>
     <row r="63" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A63" t="s">
-        <v>90</v>
+        <v>83</v>
       </c>
       <c r="B63" t="s">
-        <v>149</v>
+        <v>121</v>
       </c>
       <c r="C63" t="s">
-        <v>150</v>
+        <v>113</v>
       </c>
       <c r="D63" t="s">
-        <v>93</v>
+        <v>17</v>
       </c>
       <c r="E63" t="s">
-        <v>70</v>
+        <v>15</v>
       </c>
       <c r="F63" t="s">
-        <v>67</v>
+        <v>60</v>
       </c>
       <c r="G63" t="s">
         <v>17</v>
@@ -3451,27 +3464,27 @@
         <v>0</v>
       </c>
       <c r="I63">
-        <v>1</v>
+        <v>20</v>
       </c>
     </row>
     <row r="64" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A64" t="s">
-        <v>90</v>
+        <v>83</v>
       </c>
       <c r="B64" t="s">
-        <v>151</v>
+        <v>122</v>
       </c>
       <c r="C64" t="s">
-        <v>152</v>
+        <v>123</v>
       </c>
       <c r="D64" t="s">
-        <v>153</v>
+        <v>108</v>
       </c>
       <c r="E64" t="s">
-        <v>70</v>
+        <v>15</v>
       </c>
       <c r="F64" t="s">
-        <v>67</v>
+        <v>60</v>
       </c>
       <c r="G64" t="s">
         <v>17</v>
@@ -3479,34 +3492,34 @@
       <c r="H64">
         <v>1</v>
       </c>
-      <c r="I64" t="s">
-        <v>44</v>
+      <c r="I64">
+        <v>10000</v>
       </c>
     </row>
     <row r="65" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A65" t="s">
-        <v>90</v>
+        <v>83</v>
       </c>
       <c r="B65" t="s">
-        <v>85</v>
+        <v>124</v>
       </c>
       <c r="C65" t="s">
-        <v>154</v>
+        <v>125</v>
       </c>
       <c r="D65" t="s">
-        <v>223</v>
+        <v>216</v>
       </c>
       <c r="E65" t="s">
-        <v>52</v>
+        <v>15</v>
       </c>
       <c r="F65" t="s">
-        <v>16</v>
+        <v>60</v>
       </c>
       <c r="G65" t="s">
         <v>17</v>
       </c>
       <c r="H65">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I65">
         <v>10000</v>
@@ -3514,83 +3527,83 @@
     </row>
     <row r="66" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A66" t="s">
-        <v>90</v>
+        <v>83</v>
       </c>
       <c r="B66" t="s">
-        <v>155</v>
+        <v>126</v>
       </c>
       <c r="C66" t="s">
-        <v>156</v>
+        <v>127</v>
       </c>
       <c r="D66" t="s">
-        <v>17</v>
+        <v>128</v>
       </c>
       <c r="E66" t="s">
-        <v>52</v>
+        <v>15</v>
       </c>
       <c r="F66" t="s">
-        <v>16</v>
+        <v>60</v>
       </c>
       <c r="G66" t="s">
         <v>17</v>
       </c>
-      <c r="H66">
-        <v>0</v>
-      </c>
-      <c r="I66" t="s">
-        <v>44</v>
+      <c r="H66" s="1">
+        <v>9.9999999999999995E-7</v>
+      </c>
+      <c r="I66" s="1">
+        <v>0.01</v>
       </c>
       <c r="K66" t="s">
-        <v>157</v>
+        <v>129</v>
       </c>
     </row>
     <row r="67" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A67" t="s">
-        <v>90</v>
+        <v>83</v>
       </c>
       <c r="B67" t="s">
-        <v>86</v>
+        <v>130</v>
       </c>
       <c r="C67" t="s">
-        <v>158</v>
+        <v>131</v>
       </c>
       <c r="D67" t="s">
-        <v>225</v>
+        <v>132</v>
       </c>
       <c r="E67" t="s">
-        <v>52</v>
+        <v>15</v>
       </c>
       <c r="F67" t="s">
-        <v>16</v>
+        <v>60</v>
       </c>
       <c r="G67" t="s">
         <v>17</v>
       </c>
       <c r="H67">
-        <v>0</v>
-      </c>
-      <c r="I67" s="1">
-        <v>1000000</v>
+        <v>1</v>
+      </c>
+      <c r="I67">
+        <v>100</v>
       </c>
     </row>
     <row r="68" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A68" t="s">
-        <v>159</v>
+        <v>83</v>
       </c>
       <c r="B68" t="s">
-        <v>50</v>
+        <v>133</v>
       </c>
       <c r="C68" t="s">
-        <v>160</v>
+        <v>134</v>
       </c>
       <c r="D68" t="s">
-        <v>161</v>
+        <v>17</v>
       </c>
       <c r="E68" t="s">
-        <v>52</v>
+        <v>43</v>
       </c>
       <c r="F68" t="s">
-        <v>16</v>
+        <v>60</v>
       </c>
       <c r="G68">
         <v>1</v>
@@ -3598,31 +3611,31 @@
       <c r="H68">
         <v>0</v>
       </c>
-      <c r="I68" t="s">
-        <v>44</v>
+      <c r="I68">
+        <v>1</v>
       </c>
     </row>
     <row r="69" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A69" t="s">
-        <v>159</v>
+        <v>83</v>
       </c>
       <c r="B69" t="s">
-        <v>162</v>
+        <v>135</v>
       </c>
       <c r="C69" t="s">
-        <v>163</v>
+        <v>42</v>
       </c>
       <c r="D69" t="s">
-        <v>217</v>
+        <v>210</v>
       </c>
       <c r="E69" t="s">
-        <v>52</v>
+        <v>43</v>
       </c>
       <c r="F69" t="s">
         <v>16</v>
       </c>
-      <c r="G69">
-        <v>0</v>
+      <c r="G69" t="s">
+        <v>17</v>
       </c>
       <c r="H69">
         <v>0</v>
@@ -3633,48 +3646,48 @@
     </row>
     <row r="70" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A70" t="s">
-        <v>159</v>
+        <v>83</v>
       </c>
       <c r="B70" t="s">
-        <v>12</v>
+        <v>45</v>
       </c>
       <c r="C70" t="s">
-        <v>13</v>
+        <v>46</v>
       </c>
       <c r="D70" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="E70" t="s">
-        <v>15</v>
+        <v>43</v>
       </c>
       <c r="F70" t="s">
         <v>16</v>
       </c>
-      <c r="G70">
-        <v>1</v>
+      <c r="G70" t="s">
+        <v>17</v>
       </c>
       <c r="H70">
-        <v>0</v>
+        <v>0.1</v>
       </c>
       <c r="I70">
-        <v>4</v>
+        <v>20</v>
       </c>
     </row>
     <row r="71" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A71" t="s">
-        <v>159</v>
+        <v>83</v>
       </c>
       <c r="B71" t="s">
-        <v>41</v>
+        <v>136</v>
       </c>
       <c r="C71" t="s">
-        <v>164</v>
+        <v>137</v>
       </c>
       <c r="D71" t="s">
-        <v>217</v>
+        <v>62</v>
       </c>
       <c r="E71" t="s">
-        <v>43</v>
+        <v>63</v>
       </c>
       <c r="F71" t="s">
         <v>16</v>
@@ -3685,92 +3698,92 @@
       <c r="H71">
         <v>0</v>
       </c>
-      <c r="I71" t="s">
-        <v>44</v>
+      <c r="I71">
+        <v>100</v>
+      </c>
+      <c r="K71" t="s">
+        <v>64</v>
       </c>
     </row>
     <row r="72" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A72" t="s">
-        <v>159</v>
+        <v>83</v>
       </c>
       <c r="B72" t="s">
-        <v>45</v>
+        <v>138</v>
       </c>
       <c r="C72" t="s">
-        <v>46</v>
+        <v>139</v>
       </c>
       <c r="D72" t="s">
-        <v>17</v>
+        <v>217</v>
       </c>
       <c r="E72" t="s">
-        <v>43</v>
+        <v>63</v>
       </c>
       <c r="F72" t="s">
-        <v>16</v>
+        <v>60</v>
       </c>
       <c r="G72" t="s">
         <v>17</v>
       </c>
       <c r="H72">
-        <v>0.1</v>
+        <v>0</v>
       </c>
       <c r="I72">
-        <v>20</v>
+        <v>100000</v>
       </c>
     </row>
     <row r="73" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A73" t="s">
-        <v>159</v>
+        <v>83</v>
       </c>
       <c r="B73" t="s">
-        <v>165</v>
+        <v>140</v>
       </c>
       <c r="C73" t="s">
-        <v>166</v>
+        <v>141</v>
       </c>
       <c r="D73" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="E73" t="s">
-        <v>70</v>
+        <v>63</v>
       </c>
       <c r="F73" t="s">
-        <v>16</v>
-      </c>
-      <c r="G73" t="s">
-        <v>17</v>
+        <v>60</v>
+      </c>
+      <c r="G73">
+        <v>1</v>
       </c>
       <c r="H73">
         <v>0</v>
       </c>
       <c r="I73">
-        <v>100</v>
-      </c>
-      <c r="K73" t="s">
-        <v>167</v>
+        <v>100000</v>
       </c>
     </row>
     <row r="74" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A74" t="s">
-        <v>159</v>
+        <v>83</v>
       </c>
       <c r="B74" t="s">
-        <v>168</v>
+        <v>142</v>
       </c>
       <c r="C74" t="s">
-        <v>169</v>
+        <v>143</v>
       </c>
       <c r="D74" t="s">
-        <v>17</v>
+        <v>86</v>
       </c>
       <c r="E74" t="s">
-        <v>43</v>
+        <v>63</v>
       </c>
       <c r="F74" t="s">
-        <v>16</v>
-      </c>
-      <c r="G74">
-        <v>0</v>
+        <v>60</v>
+      </c>
+      <c r="G74" t="s">
+        <v>17</v>
       </c>
       <c r="H74">
         <v>0</v>
@@ -3778,124 +3791,118 @@
       <c r="I74">
         <v>1</v>
       </c>
-      <c r="K74" t="s">
-        <v>170</v>
-      </c>
     </row>
     <row r="75" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A75" t="s">
-        <v>159</v>
+        <v>83</v>
       </c>
       <c r="B75" t="s">
-        <v>171</v>
+        <v>144</v>
       </c>
       <c r="C75" t="s">
-        <v>172</v>
+        <v>145</v>
       </c>
       <c r="D75" t="s">
-        <v>17</v>
+        <v>146</v>
       </c>
       <c r="E75" t="s">
-        <v>70</v>
+        <v>63</v>
       </c>
       <c r="F75" t="s">
-        <v>16</v>
-      </c>
-      <c r="G75">
-        <v>0</v>
+        <v>60</v>
+      </c>
+      <c r="G75" t="s">
+        <v>17</v>
       </c>
       <c r="H75">
-        <v>0</v>
-      </c>
-      <c r="I75">
         <v>1</v>
       </c>
-      <c r="K75" t="s">
-        <v>170</v>
+      <c r="I75" t="s">
+        <v>44</v>
       </c>
     </row>
     <row r="76" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A76" t="s">
-        <v>159</v>
+        <v>83</v>
       </c>
       <c r="B76" t="s">
-        <v>173</v>
+        <v>78</v>
       </c>
       <c r="C76" t="s">
-        <v>174</v>
+        <v>147</v>
       </c>
       <c r="D76" t="s">
-        <v>93</v>
+        <v>216</v>
       </c>
       <c r="E76" t="s">
-        <v>15</v>
+        <v>49</v>
       </c>
       <c r="F76" t="s">
         <v>16</v>
       </c>
-      <c r="G76">
-        <v>0</v>
+      <c r="G76" t="s">
+        <v>17</v>
       </c>
       <c r="H76">
         <v>0</v>
       </c>
       <c r="I76">
-        <v>1</v>
-      </c>
-      <c r="K76" t="s">
-        <v>175</v>
+        <v>10000</v>
       </c>
     </row>
     <row r="77" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A77" t="s">
-        <v>176</v>
+        <v>83</v>
       </c>
       <c r="B77" t="s">
-        <v>85</v>
+        <v>148</v>
       </c>
       <c r="C77" t="s">
-        <v>51</v>
+        <v>149</v>
       </c>
       <c r="D77" t="s">
-        <v>220</v>
+        <v>17</v>
       </c>
       <c r="E77" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="F77" t="s">
         <v>16</v>
       </c>
-      <c r="G77">
-        <v>1.1999999999999999E-3</v>
+      <c r="G77" t="s">
+        <v>17</v>
       </c>
       <c r="H77">
         <v>0</v>
       </c>
-      <c r="I77">
-        <v>1000</v>
+      <c r="I77" t="s">
+        <v>44</v>
+      </c>
+      <c r="K77" t="s">
+        <v>150</v>
       </c>
     </row>
     <row r="78" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A78" t="s">
-        <v>176</v>
+        <v>83</v>
       </c>
       <c r="B78" t="s">
-        <v>86</v>
+        <v>79</v>
       </c>
       <c r="C78" t="s">
-        <v>87</v>
+        <v>151</v>
       </c>
       <c r="D78" t="s">
-        <v>221</v>
+        <v>218</v>
       </c>
       <c r="E78" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="F78" t="s">
         <v>16</v>
       </c>
-      <c r="G78">
-        <v>0</v>
+      <c r="G78" t="s">
+        <v>17</v>
       </c>
       <c r="H78">
         <v>0</v>
@@ -3906,80 +3913,71 @@
     </row>
     <row r="79" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A79" t="s">
-        <v>176</v>
+        <v>152</v>
       </c>
       <c r="B79" t="s">
-        <v>177</v>
+        <v>47</v>
       </c>
       <c r="C79" t="s">
-        <v>178</v>
+        <v>153</v>
       </c>
       <c r="D79" t="s">
-        <v>93</v>
+        <v>154</v>
       </c>
       <c r="E79" t="s">
-        <v>15</v>
+        <v>49</v>
       </c>
       <c r="F79" t="s">
-        <v>67</v>
-      </c>
-      <c r="G79" t="b">
+        <v>16</v>
+      </c>
+      <c r="G79">
         <v>1</v>
       </c>
       <c r="H79">
         <v>0</v>
       </c>
-      <c r="I79">
-        <v>1</v>
-      </c>
-      <c r="J79" t="s">
-        <v>179</v>
-      </c>
-      <c r="K79" t="s">
-        <v>180</v>
+      <c r="I79" t="s">
+        <v>44</v>
       </c>
     </row>
     <row r="80" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A80" t="s">
-        <v>176</v>
+        <v>152</v>
       </c>
       <c r="B80" t="s">
-        <v>60</v>
+        <v>155</v>
       </c>
       <c r="C80" t="s">
-        <v>61</v>
+        <v>156</v>
       </c>
       <c r="D80" t="s">
-        <v>14</v>
+        <v>210</v>
       </c>
       <c r="E80" t="s">
-        <v>15</v>
+        <v>49</v>
       </c>
       <c r="F80" t="s">
         <v>16</v>
       </c>
       <c r="G80">
-        <v>0.42</v>
+        <v>0</v>
       </c>
       <c r="H80">
         <v>0</v>
       </c>
-      <c r="I80">
-        <v>1</v>
-      </c>
-      <c r="K80" t="s">
-        <v>181</v>
+      <c r="I80" t="s">
+        <v>44</v>
       </c>
     </row>
     <row r="81" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A81" t="s">
-        <v>176</v>
+        <v>152</v>
       </c>
       <c r="B81" t="s">
-        <v>99</v>
+        <v>12</v>
       </c>
       <c r="C81" t="s">
-        <v>100</v>
+        <v>13</v>
       </c>
       <c r="D81" t="s">
         <v>14</v>
@@ -3988,532 +3986,544 @@
         <v>15</v>
       </c>
       <c r="F81" t="s">
-        <v>67</v>
+        <v>16</v>
       </c>
       <c r="G81">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H81">
         <v>0</v>
       </c>
       <c r="I81">
-        <v>3</v>
-      </c>
-      <c r="K81" t="s">
-        <v>182</v>
+        <v>4</v>
       </c>
     </row>
     <row r="82" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A82" t="s">
-        <v>176</v>
+        <v>152</v>
       </c>
       <c r="B82" t="s">
-        <v>183</v>
+        <v>41</v>
       </c>
       <c r="C82" t="s">
-        <v>184</v>
+        <v>157</v>
       </c>
       <c r="D82" t="s">
-        <v>220</v>
+        <v>210</v>
       </c>
       <c r="E82" t="s">
-        <v>15</v>
+        <v>43</v>
       </c>
       <c r="F82" t="s">
-        <v>67</v>
-      </c>
-      <c r="G82" s="1">
-        <v>5.0000000000000001E-4</v>
+        <v>16</v>
+      </c>
+      <c r="G82" t="s">
+        <v>17</v>
       </c>
       <c r="H82">
         <v>0</v>
       </c>
-      <c r="I82" s="1">
-        <v>0.1</v>
+      <c r="I82" t="s">
+        <v>44</v>
       </c>
     </row>
     <row r="83" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A83" t="s">
-        <v>176</v>
+        <v>152</v>
       </c>
       <c r="B83" t="s">
-        <v>33</v>
+        <v>45</v>
       </c>
       <c r="C83" t="s">
-        <v>104</v>
+        <v>46</v>
       </c>
       <c r="D83" t="s">
-        <v>211</v>
+        <v>17</v>
       </c>
       <c r="E83" t="s">
-        <v>15</v>
+        <v>43</v>
       </c>
       <c r="F83" t="s">
-        <v>67</v>
-      </c>
-      <c r="G83">
-        <v>26.7</v>
+        <v>16</v>
+      </c>
+      <c r="G83" t="s">
+        <v>17</v>
       </c>
       <c r="H83">
-        <v>4</v>
+        <v>0.1</v>
       </c>
       <c r="I83">
-        <v>40</v>
+        <v>20</v>
       </c>
     </row>
     <row r="84" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A84" t="s">
-        <v>176</v>
+        <v>152</v>
       </c>
       <c r="B84" t="s">
-        <v>35</v>
+        <v>158</v>
       </c>
       <c r="C84" t="s">
-        <v>36</v>
+        <v>159</v>
       </c>
       <c r="D84" t="s">
-        <v>211</v>
+        <v>14</v>
       </c>
       <c r="E84" t="s">
-        <v>15</v>
+        <v>63</v>
       </c>
       <c r="F84" t="s">
-        <v>67</v>
-      </c>
-      <c r="G84">
-        <v>8</v>
+        <v>16</v>
+      </c>
+      <c r="G84" t="s">
+        <v>17</v>
       </c>
       <c r="H84">
         <v>0</v>
       </c>
       <c r="I84">
-        <v>40</v>
+        <v>100</v>
+      </c>
+      <c r="K84" t="s">
+        <v>160</v>
       </c>
     </row>
     <row r="85" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A85" t="s">
-        <v>176</v>
+        <v>152</v>
       </c>
       <c r="B85" t="s">
-        <v>37</v>
+        <v>161</v>
       </c>
       <c r="C85" t="s">
-        <v>38</v>
+        <v>162</v>
       </c>
       <c r="D85" t="s">
-        <v>211</v>
+        <v>17</v>
       </c>
       <c r="E85" t="s">
-        <v>15</v>
+        <v>43</v>
       </c>
       <c r="F85" t="s">
-        <v>67</v>
+        <v>16</v>
       </c>
       <c r="G85">
-        <v>40.5</v>
+        <v>0</v>
       </c>
       <c r="H85">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="I85">
-        <v>50</v>
+        <v>1</v>
+      </c>
+      <c r="K85" t="s">
+        <v>163</v>
       </c>
     </row>
     <row r="86" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A86" t="s">
-        <v>176</v>
+        <v>152</v>
       </c>
       <c r="B86" t="s">
-        <v>107</v>
+        <v>164</v>
       </c>
       <c r="C86" t="s">
-        <v>185</v>
+        <v>165</v>
       </c>
       <c r="D86" t="s">
         <v>17</v>
       </c>
       <c r="E86" t="s">
-        <v>15</v>
+        <v>63</v>
       </c>
       <c r="F86" t="s">
-        <v>67</v>
+        <v>16</v>
       </c>
       <c r="G86">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="H86">
         <v>0</v>
       </c>
       <c r="I86">
-        <v>10</v>
+        <v>1</v>
+      </c>
+      <c r="K86" t="s">
+        <v>163</v>
       </c>
     </row>
     <row r="87" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A87" t="s">
-        <v>176</v>
+        <v>152</v>
       </c>
       <c r="B87" t="s">
-        <v>186</v>
+        <v>166</v>
       </c>
       <c r="C87" t="s">
-        <v>106</v>
+        <v>167</v>
       </c>
       <c r="D87" t="s">
-        <v>211</v>
+        <v>86</v>
       </c>
       <c r="E87" t="s">
         <v>15</v>
       </c>
       <c r="F87" t="s">
-        <v>67</v>
+        <v>16</v>
       </c>
       <c r="G87">
-        <v>25</v>
+        <v>0</v>
       </c>
       <c r="H87">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="I87">
-        <v>40</v>
+        <v>1</v>
+      </c>
+      <c r="K87" t="s">
+        <v>168</v>
       </c>
     </row>
     <row r="88" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A88" t="s">
-        <v>176</v>
+        <v>169</v>
       </c>
       <c r="B88" t="s">
-        <v>187</v>
+        <v>78</v>
       </c>
       <c r="C88" t="s">
-        <v>188</v>
+        <v>48</v>
       </c>
       <c r="D88" t="s">
-        <v>226</v>
+        <v>213</v>
       </c>
       <c r="E88" t="s">
-        <v>15</v>
+        <v>49</v>
       </c>
       <c r="F88" t="s">
-        <v>67</v>
-      </c>
-      <c r="G88" s="1">
-        <v>5.0000000000000002E-5</v>
-      </c>
-      <c r="H88" s="1">
-        <v>1E-10</v>
+        <v>16</v>
+      </c>
+      <c r="G88">
+        <v>1.1999999999999999E-3</v>
+      </c>
+      <c r="H88">
+        <v>0</v>
       </c>
       <c r="I88">
-        <v>1</v>
-      </c>
-      <c r="K88" t="s">
-        <v>189</v>
+        <v>1000</v>
       </c>
     </row>
     <row r="89" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A89" t="s">
-        <v>176</v>
+        <v>169</v>
       </c>
       <c r="B89" t="s">
-        <v>190</v>
+        <v>79</v>
       </c>
       <c r="C89" t="s">
-        <v>191</v>
+        <v>80</v>
       </c>
       <c r="D89" t="s">
-        <v>17</v>
+        <v>214</v>
       </c>
       <c r="E89" t="s">
-        <v>15</v>
+        <v>49</v>
       </c>
       <c r="F89" t="s">
-        <v>67</v>
+        <v>16</v>
       </c>
       <c r="G89">
-        <v>2.5000000000000001E-2</v>
-      </c>
-      <c r="H89" s="1">
-        <v>1E-10</v>
-      </c>
-      <c r="I89">
-        <v>1</v>
-      </c>
-      <c r="K89" t="s">
-        <v>189</v>
+        <v>0</v>
+      </c>
+      <c r="H89">
+        <v>0</v>
+      </c>
+      <c r="I89" s="1">
+        <v>1000000</v>
       </c>
     </row>
     <row r="90" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A90" t="s">
-        <v>176</v>
+        <v>169</v>
       </c>
       <c r="B90" t="s">
-        <v>192</v>
+        <v>170</v>
       </c>
       <c r="C90" t="s">
-        <v>193</v>
+        <v>171</v>
       </c>
       <c r="D90" t="s">
-        <v>194</v>
+        <v>86</v>
       </c>
       <c r="E90" t="s">
         <v>15</v>
       </c>
       <c r="F90" t="s">
-        <v>67</v>
-      </c>
-      <c r="G90">
-        <v>3.4000000000000002E-2</v>
+        <v>60</v>
+      </c>
+      <c r="G90" t="b">
+        <v>1</v>
       </c>
       <c r="H90">
         <v>0</v>
       </c>
       <c r="I90">
-        <v>10</v>
+        <v>1</v>
+      </c>
+      <c r="J90" t="s">
+        <v>172</v>
+      </c>
+      <c r="K90" t="s">
+        <v>173</v>
       </c>
     </row>
     <row r="91" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A91" t="s">
-        <v>176</v>
+        <v>169</v>
       </c>
       <c r="B91" t="s">
-        <v>195</v>
+        <v>54</v>
       </c>
       <c r="C91" t="s">
-        <v>196</v>
+        <v>55</v>
       </c>
       <c r="D91" t="s">
-        <v>24</v>
+        <v>14</v>
       </c>
       <c r="E91" t="s">
         <v>15</v>
       </c>
       <c r="F91" t="s">
-        <v>67</v>
+        <v>16</v>
       </c>
       <c r="G91">
-        <v>4.3E-3</v>
+        <v>0.42</v>
       </c>
       <c r="H91">
         <v>0</v>
       </c>
       <c r="I91">
-        <v>10</v>
+        <v>1</v>
+      </c>
+      <c r="K91" t="s">
+        <v>174</v>
       </c>
     </row>
     <row r="92" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A92" t="s">
-        <v>176</v>
+        <v>169</v>
       </c>
       <c r="B92" t="s">
-        <v>88</v>
+        <v>92</v>
       </c>
       <c r="C92" t="s">
-        <v>89</v>
+        <v>93</v>
       </c>
       <c r="D92" t="s">
-        <v>227</v>
+        <v>14</v>
       </c>
       <c r="E92" t="s">
         <v>15</v>
       </c>
       <c r="F92" t="s">
-        <v>67</v>
+        <v>60</v>
       </c>
       <c r="G92">
-        <v>177</v>
+        <v>0</v>
       </c>
       <c r="H92">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I92">
-        <v>10000</v>
+        <v>3</v>
+      </c>
+      <c r="K92" t="s">
+        <v>175</v>
       </c>
     </row>
     <row r="93" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A93" t="s">
+        <v>169</v>
+      </c>
+      <c r="B93" t="s">
         <v>176</v>
       </c>
-      <c r="B93" t="s">
-        <v>65</v>
-      </c>
       <c r="C93" t="s">
-        <v>141</v>
+        <v>177</v>
       </c>
       <c r="D93" t="s">
-        <v>17</v>
+        <v>213</v>
       </c>
       <c r="E93" t="s">
-        <v>43</v>
+        <v>15</v>
       </c>
       <c r="F93" t="s">
-        <v>67</v>
-      </c>
-      <c r="G93">
-        <v>1</v>
+        <v>60</v>
+      </c>
+      <c r="G93" s="1">
+        <v>5.0000000000000001E-4</v>
       </c>
       <c r="H93">
         <v>0</v>
       </c>
-      <c r="I93">
-        <v>1</v>
+      <c r="I93" s="1">
+        <v>0.1</v>
       </c>
     </row>
     <row r="94" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A94" t="s">
-        <v>176</v>
+        <v>169</v>
       </c>
       <c r="B94" t="s">
-        <v>63</v>
+        <v>33</v>
       </c>
       <c r="C94" t="s">
-        <v>42</v>
+        <v>97</v>
       </c>
       <c r="D94" t="s">
-        <v>217</v>
+        <v>204</v>
       </c>
       <c r="E94" t="s">
-        <v>43</v>
+        <v>15</v>
       </c>
       <c r="F94" t="s">
-        <v>16</v>
-      </c>
-      <c r="G94" t="s">
-        <v>197</v>
+        <v>60</v>
+      </c>
+      <c r="G94">
+        <v>26.7</v>
       </c>
       <c r="H94">
-        <v>0</v>
-      </c>
-      <c r="I94" t="s">
-        <v>44</v>
+        <v>4</v>
+      </c>
+      <c r="I94">
+        <v>40</v>
       </c>
     </row>
     <row r="95" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A95" t="s">
-        <v>176</v>
+        <v>169</v>
       </c>
       <c r="B95" t="s">
-        <v>45</v>
+        <v>35</v>
       </c>
       <c r="C95" t="s">
-        <v>46</v>
+        <v>36</v>
       </c>
       <c r="D95" t="s">
-        <v>17</v>
+        <v>204</v>
       </c>
       <c r="E95" t="s">
-        <v>43</v>
+        <v>15</v>
       </c>
       <c r="F95" t="s">
-        <v>16</v>
-      </c>
-      <c r="G95" t="s">
-        <v>197</v>
+        <v>60</v>
+      </c>
+      <c r="G95">
+        <v>8</v>
       </c>
       <c r="H95">
-        <v>0.1</v>
+        <v>0</v>
       </c>
       <c r="I95">
-        <v>20</v>
+        <v>40</v>
       </c>
     </row>
     <row r="96" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A96" t="s">
-        <v>176</v>
+        <v>169</v>
       </c>
       <c r="B96" t="s">
-        <v>55</v>
+        <v>37</v>
       </c>
       <c r="C96" t="s">
-        <v>198</v>
+        <v>38</v>
       </c>
       <c r="D96" t="s">
-        <v>69</v>
+        <v>204</v>
       </c>
       <c r="E96" t="s">
-        <v>70</v>
+        <v>15</v>
       </c>
       <c r="F96" t="s">
-        <v>16</v>
-      </c>
-      <c r="G96" t="s">
-        <v>17</v>
+        <v>60</v>
+      </c>
+      <c r="G96">
+        <v>40.5</v>
       </c>
       <c r="H96">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="I96">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="97" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A97" t="s">
+        <v>169</v>
+      </c>
+      <c r="B97" t="s">
         <v>100</v>
       </c>
-      <c r="K96" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="97" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A97" t="s">
-        <v>176</v>
-      </c>
-      <c r="B97" t="s">
-        <v>72</v>
-      </c>
       <c r="C97" t="s">
-        <v>73</v>
+        <v>178</v>
       </c>
       <c r="D97" t="s">
-        <v>218</v>
+        <v>17</v>
       </c>
       <c r="E97" t="s">
         <v>15</v>
       </c>
       <c r="F97" t="s">
-        <v>67</v>
+        <v>60</v>
       </c>
       <c r="G97">
-        <v>1000</v>
+        <v>2</v>
       </c>
       <c r="H97">
-        <v>100</v>
+        <v>0</v>
       </c>
       <c r="I97">
-        <v>10000</v>
-      </c>
-    </row>
-    <row r="98" spans="1:9" x14ac:dyDescent="0.3">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="98" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A98" t="s">
-        <v>176</v>
+        <v>169</v>
       </c>
       <c r="B98" t="s">
-        <v>74</v>
+        <v>179</v>
       </c>
       <c r="C98" t="s">
-        <v>75</v>
+        <v>99</v>
       </c>
       <c r="D98" t="s">
-        <v>17</v>
+        <v>204</v>
       </c>
       <c r="E98" t="s">
         <v>15</v>
       </c>
       <c r="F98" t="s">
-        <v>67</v>
+        <v>60</v>
       </c>
       <c r="G98">
-        <v>16.7</v>
+        <v>25</v>
       </c>
       <c r="H98">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="I98">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="99" spans="1:9" x14ac:dyDescent="0.3">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="99" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A99" t="s">
-        <v>176</v>
+        <v>169</v>
       </c>
       <c r="B99" t="s">
-        <v>76</v>
+        <v>180</v>
       </c>
       <c r="C99" t="s">
-        <v>77</v>
+        <v>181</v>
       </c>
       <c r="D99" t="s">
         <v>219</v>
@@ -4522,439 +4532,448 @@
         <v>15</v>
       </c>
       <c r="F99" t="s">
+        <v>60</v>
+      </c>
+      <c r="G99" s="1">
+        <v>5.0000000000000002E-5</v>
+      </c>
+      <c r="H99" s="1">
+        <v>1E-10</v>
+      </c>
+      <c r="I99">
+        <v>1</v>
+      </c>
+      <c r="K99" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="100" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A100" t="s">
+        <v>169</v>
+      </c>
+      <c r="B100" t="s">
+        <v>183</v>
+      </c>
+      <c r="C100" t="s">
+        <v>184</v>
+      </c>
+      <c r="D100" t="s">
+        <v>17</v>
+      </c>
+      <c r="E100" t="s">
+        <v>15</v>
+      </c>
+      <c r="F100" t="s">
+        <v>60</v>
+      </c>
+      <c r="G100">
+        <v>0.25</v>
+      </c>
+      <c r="H100" s="1">
+        <v>1E-10</v>
+      </c>
+      <c r="I100">
+        <v>1</v>
+      </c>
+      <c r="K100" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="101" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A101" t="s">
+        <v>169</v>
+      </c>
+      <c r="B101" t="s">
+        <v>185</v>
+      </c>
+      <c r="C101" t="s">
+        <v>186</v>
+      </c>
+      <c r="D101" t="s">
+        <v>187</v>
+      </c>
+      <c r="E101" t="s">
+        <v>15</v>
+      </c>
+      <c r="F101" t="s">
+        <v>60</v>
+      </c>
+      <c r="G101">
+        <v>3.4000000000000002E-2</v>
+      </c>
+      <c r="H101">
+        <v>0</v>
+      </c>
+      <c r="I101">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="102" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A102" t="s">
+        <v>169</v>
+      </c>
+      <c r="B102" t="s">
+        <v>188</v>
+      </c>
+      <c r="C102" t="s">
+        <v>189</v>
+      </c>
+      <c r="D102" t="s">
+        <v>24</v>
+      </c>
+      <c r="E102" t="s">
+        <v>15</v>
+      </c>
+      <c r="F102" t="s">
+        <v>60</v>
+      </c>
+      <c r="G102">
+        <v>4.3E-3</v>
+      </c>
+      <c r="H102">
+        <v>0</v>
+      </c>
+      <c r="I102">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="103" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A103" t="s">
+        <v>169</v>
+      </c>
+      <c r="B103" t="s">
+        <v>81</v>
+      </c>
+      <c r="C103" t="s">
+        <v>82</v>
+      </c>
+      <c r="D103" t="s">
+        <v>220</v>
+      </c>
+      <c r="E103" t="s">
+        <v>15</v>
+      </c>
+      <c r="F103" t="s">
+        <v>60</v>
+      </c>
+      <c r="G103">
+        <v>177</v>
+      </c>
+      <c r="H103">
+        <v>1</v>
+      </c>
+      <c r="I103">
+        <v>10000</v>
+      </c>
+    </row>
+    <row r="104" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A104" t="s">
+        <v>169</v>
+      </c>
+      <c r="B104" t="s">
+        <v>58</v>
+      </c>
+      <c r="C104" t="s">
+        <v>134</v>
+      </c>
+      <c r="D104" t="s">
+        <v>17</v>
+      </c>
+      <c r="E104" t="s">
+        <v>43</v>
+      </c>
+      <c r="F104" t="s">
+        <v>60</v>
+      </c>
+      <c r="G104">
+        <v>1</v>
+      </c>
+      <c r="H104">
+        <v>0</v>
+      </c>
+      <c r="I104">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="105" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A105" t="s">
+        <v>169</v>
+      </c>
+      <c r="B105" t="s">
+        <v>56</v>
+      </c>
+      <c r="C105" t="s">
+        <v>42</v>
+      </c>
+      <c r="D105" t="s">
+        <v>210</v>
+      </c>
+      <c r="E105" t="s">
+        <v>43</v>
+      </c>
+      <c r="F105" t="s">
+        <v>16</v>
+      </c>
+      <c r="G105" t="s">
+        <v>190</v>
+      </c>
+      <c r="H105">
+        <v>0</v>
+      </c>
+      <c r="I105" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="106" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A106" t="s">
+        <v>169</v>
+      </c>
+      <c r="B106" t="s">
+        <v>45</v>
+      </c>
+      <c r="C106" t="s">
+        <v>46</v>
+      </c>
+      <c r="D106" t="s">
+        <v>17</v>
+      </c>
+      <c r="E106" t="s">
+        <v>43</v>
+      </c>
+      <c r="F106" t="s">
+        <v>16</v>
+      </c>
+      <c r="G106" t="s">
+        <v>190</v>
+      </c>
+      <c r="H106">
+        <v>0.1</v>
+      </c>
+      <c r="I106">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="107" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A107" t="s">
+        <v>169</v>
+      </c>
+      <c r="B107" t="s">
+        <v>52</v>
+      </c>
+      <c r="C107" t="s">
+        <v>191</v>
+      </c>
+      <c r="D107" t="s">
+        <v>62</v>
+      </c>
+      <c r="E107" t="s">
+        <v>63</v>
+      </c>
+      <c r="F107" t="s">
+        <v>16</v>
+      </c>
+      <c r="G107" t="s">
+        <v>17</v>
+      </c>
+      <c r="H107">
+        <v>0</v>
+      </c>
+      <c r="I107">
+        <v>100</v>
+      </c>
+      <c r="K107" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="108" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A108" t="s">
+        <v>169</v>
+      </c>
+      <c r="B108" t="s">
+        <v>65</v>
+      </c>
+      <c r="C108" t="s">
+        <v>66</v>
+      </c>
+      <c r="D108" t="s">
+        <v>211</v>
+      </c>
+      <c r="E108" t="s">
+        <v>15</v>
+      </c>
+      <c r="F108" t="s">
+        <v>60</v>
+      </c>
+      <c r="G108">
+        <v>1000</v>
+      </c>
+      <c r="H108">
+        <v>100</v>
+      </c>
+      <c r="I108">
+        <v>10000</v>
+      </c>
+    </row>
+    <row r="109" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A109" t="s">
+        <v>169</v>
+      </c>
+      <c r="B109" t="s">
         <v>67</v>
       </c>
-      <c r="G99">
+      <c r="C109" t="s">
+        <v>68</v>
+      </c>
+      <c r="D109" t="s">
+        <v>17</v>
+      </c>
+      <c r="E109" t="s">
+        <v>15</v>
+      </c>
+      <c r="F109" t="s">
+        <v>60</v>
+      </c>
+      <c r="G109">
+        <v>16.7</v>
+      </c>
+      <c r="H109">
+        <v>5</v>
+      </c>
+      <c r="I109">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="110" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A110" t="s">
+        <v>169</v>
+      </c>
+      <c r="B110" t="s">
+        <v>69</v>
+      </c>
+      <c r="C110" t="s">
+        <v>70</v>
+      </c>
+      <c r="D110" t="s">
+        <v>212</v>
+      </c>
+      <c r="E110" t="s">
+        <v>15</v>
+      </c>
+      <c r="F110" t="s">
+        <v>60</v>
+      </c>
+      <c r="G110">
         <v>1</v>
       </c>
-      <c r="H99">
+      <c r="H110">
         <v>0.5</v>
       </c>
-      <c r="I99">
+      <c r="I110">
         <v>1.5</v>
       </c>
     </row>
-    <row r="100" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A100" t="s">
-        <v>176</v>
-      </c>
-      <c r="B100" t="s">
-        <v>199</v>
-      </c>
-      <c r="C100" t="s">
-        <v>200</v>
-      </c>
-      <c r="D100" t="s">
-        <v>201</v>
-      </c>
-      <c r="E100" t="s">
-        <v>15</v>
-      </c>
-      <c r="F100" t="s">
-        <v>67</v>
-      </c>
-      <c r="G100" s="1">
+    <row r="111" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A111" t="s">
+        <v>169</v>
+      </c>
+      <c r="B111" t="s">
+        <v>192</v>
+      </c>
+      <c r="C111" t="s">
+        <v>193</v>
+      </c>
+      <c r="D111" t="s">
+        <v>194</v>
+      </c>
+      <c r="E111" t="s">
+        <v>15</v>
+      </c>
+      <c r="F111" t="s">
+        <v>60</v>
+      </c>
+      <c r="G111" s="1">
         <v>1E-4</v>
       </c>
-      <c r="H100">
-        <v>0</v>
-      </c>
-      <c r="I100">
+      <c r="H111">
+        <v>0</v>
+      </c>
+      <c r="I111">
         <v>0.1</v>
       </c>
     </row>
-    <row r="101" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A101" t="s">
-        <v>176</v>
-      </c>
-      <c r="B101" t="s">
-        <v>81</v>
-      </c>
-      <c r="C101" t="s">
-        <v>82</v>
-      </c>
-      <c r="D101" t="s">
-        <v>17</v>
-      </c>
-      <c r="E101" t="s">
-        <v>70</v>
-      </c>
-      <c r="F101" t="s">
-        <v>16</v>
-      </c>
-      <c r="G101">
+    <row r="112" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A112" t="s">
+        <v>169</v>
+      </c>
+      <c r="B112" t="s">
+        <v>74</v>
+      </c>
+      <c r="C112" t="s">
+        <v>75</v>
+      </c>
+      <c r="D112" t="s">
+        <v>17</v>
+      </c>
+      <c r="E112" t="s">
+        <v>63</v>
+      </c>
+      <c r="F112" t="s">
+        <v>16</v>
+      </c>
+      <c r="G112">
         <v>1</v>
       </c>
-      <c r="H101">
-        <v>0</v>
-      </c>
-      <c r="I101">
+      <c r="H112">
+        <v>0</v>
+      </c>
+      <c r="I112">
         <v>100000</v>
-      </c>
-    </row>
-    <row r="102" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A102" t="s">
-        <v>176</v>
-      </c>
-      <c r="B102" t="s">
-        <v>83</v>
-      </c>
-      <c r="C102" t="s">
-        <v>84</v>
-      </c>
-      <c r="D102" t="s">
-        <v>14</v>
-      </c>
-      <c r="E102" t="s">
-        <v>70</v>
-      </c>
-      <c r="F102" t="s">
-        <v>67</v>
-      </c>
-      <c r="G102">
-        <v>0</v>
-      </c>
-      <c r="H102">
-        <v>0</v>
-      </c>
-      <c r="I102">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="103" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A103" t="s">
-        <v>202</v>
-      </c>
-      <c r="B103" t="s">
-        <v>12</v>
-      </c>
-      <c r="C103" t="s">
-        <v>13</v>
-      </c>
-      <c r="D103" t="s">
-        <v>14</v>
-      </c>
-      <c r="E103" t="s">
-        <v>15</v>
-      </c>
-      <c r="F103" t="s">
-        <v>16</v>
-      </c>
-      <c r="G103" t="s">
-        <v>17</v>
-      </c>
-      <c r="H103">
-        <v>0</v>
-      </c>
-      <c r="I103">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="104" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A104" t="s">
-        <v>202</v>
-      </c>
-      <c r="B104" t="s">
-        <v>18</v>
-      </c>
-      <c r="C104" t="s">
-        <v>19</v>
-      </c>
-      <c r="D104" t="s">
-        <v>14</v>
-      </c>
-      <c r="E104" t="s">
-        <v>15</v>
-      </c>
-      <c r="F104" t="s">
-        <v>16</v>
-      </c>
-      <c r="G104" t="s">
-        <v>17</v>
-      </c>
-      <c r="H104">
-        <v>0</v>
-      </c>
-      <c r="I104">
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="105" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A105" t="s">
-        <v>202</v>
-      </c>
-      <c r="B105" t="s">
-        <v>20</v>
-      </c>
-      <c r="C105" t="s">
-        <v>21</v>
-      </c>
-      <c r="D105" t="s">
-        <v>207</v>
-      </c>
-      <c r="E105" t="s">
-        <v>15</v>
-      </c>
-      <c r="F105" t="s">
-        <v>16</v>
-      </c>
-      <c r="G105" t="s">
-        <v>17</v>
-      </c>
-      <c r="H105" s="1">
-        <v>9.9999999999999995E-7</v>
-      </c>
-      <c r="I105">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="106" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A106" t="s">
-        <v>202</v>
-      </c>
-      <c r="B106" t="s">
-        <v>22</v>
-      </c>
-      <c r="C106" t="s">
-        <v>23</v>
-      </c>
-      <c r="D106" t="s">
-        <v>24</v>
-      </c>
-      <c r="E106" t="s">
-        <v>15</v>
-      </c>
-      <c r="F106" t="s">
-        <v>16</v>
-      </c>
-      <c r="G106" t="s">
-        <v>17</v>
-      </c>
-      <c r="H106">
-        <v>0</v>
-      </c>
-      <c r="I106">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="107" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A107" t="s">
-        <v>202</v>
-      </c>
-      <c r="B107" t="s">
-        <v>25</v>
-      </c>
-      <c r="C107" t="s">
-        <v>26</v>
-      </c>
-      <c r="D107" t="s">
-        <v>209</v>
-      </c>
-      <c r="E107" t="s">
-        <v>15</v>
-      </c>
-      <c r="F107" t="s">
-        <v>16</v>
-      </c>
-      <c r="G107" t="s">
-        <v>17</v>
-      </c>
-      <c r="H107" s="1">
-        <v>9.9999999999999995E-7</v>
-      </c>
-      <c r="I107">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="108" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A108" t="s">
-        <v>202</v>
-      </c>
-      <c r="B108" t="s">
-        <v>27</v>
-      </c>
-      <c r="C108" t="s">
-        <v>28</v>
-      </c>
-      <c r="D108" t="s">
-        <v>209</v>
-      </c>
-      <c r="E108" t="s">
-        <v>15</v>
-      </c>
-      <c r="F108" t="s">
-        <v>16</v>
-      </c>
-      <c r="G108" t="s">
-        <v>17</v>
-      </c>
-      <c r="H108" s="1">
-        <v>1E-4</v>
-      </c>
-      <c r="I108">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="109" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A109" t="s">
-        <v>202</v>
-      </c>
-      <c r="B109" t="s">
-        <v>33</v>
-      </c>
-      <c r="C109" t="s">
-        <v>34</v>
-      </c>
-      <c r="D109" t="s">
-        <v>211</v>
-      </c>
-      <c r="E109" t="s">
-        <v>15</v>
-      </c>
-      <c r="F109" t="s">
-        <v>16</v>
-      </c>
-      <c r="G109" t="s">
-        <v>17</v>
-      </c>
-      <c r="H109">
-        <v>4</v>
-      </c>
-      <c r="I109">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="110" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A110" t="s">
-        <v>202</v>
-      </c>
-      <c r="B110" t="s">
-        <v>35</v>
-      </c>
-      <c r="C110" t="s">
-        <v>36</v>
-      </c>
-      <c r="D110" t="s">
-        <v>211</v>
-      </c>
-      <c r="E110" t="s">
-        <v>15</v>
-      </c>
-      <c r="F110" t="s">
-        <v>16</v>
-      </c>
-      <c r="G110" t="s">
-        <v>17</v>
-      </c>
-      <c r="H110">
-        <v>0</v>
-      </c>
-      <c r="I110">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="111" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A111" t="s">
-        <v>202</v>
-      </c>
-      <c r="B111" t="s">
-        <v>37</v>
-      </c>
-      <c r="C111" t="s">
-        <v>38</v>
-      </c>
-      <c r="D111" t="s">
-        <v>211</v>
-      </c>
-      <c r="E111" t="s">
-        <v>15</v>
-      </c>
-      <c r="F111" t="s">
-        <v>16</v>
-      </c>
-      <c r="G111" t="s">
-        <v>17</v>
-      </c>
-      <c r="H111">
-        <v>10</v>
-      </c>
-      <c r="I111">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="112" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A112" t="s">
-        <v>202</v>
-      </c>
-      <c r="B112" t="s">
-        <v>39</v>
-      </c>
-      <c r="C112" t="s">
-        <v>40</v>
-      </c>
-      <c r="D112" t="s">
-        <v>212</v>
-      </c>
-      <c r="E112" t="s">
-        <v>15</v>
-      </c>
-      <c r="F112" t="s">
-        <v>16</v>
-      </c>
-      <c r="G112" t="s">
-        <v>17</v>
-      </c>
-      <c r="H112">
-        <v>20</v>
-      </c>
-      <c r="I112">
-        <v>300</v>
       </c>
     </row>
     <row r="113" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A113" t="s">
-        <v>202</v>
+        <v>169</v>
       </c>
       <c r="B113" t="s">
-        <v>41</v>
+        <v>76</v>
       </c>
       <c r="C113" t="s">
-        <v>42</v>
+        <v>77</v>
       </c>
       <c r="D113" t="s">
-        <v>213</v>
+        <v>14</v>
       </c>
       <c r="E113" t="s">
-        <v>43</v>
+        <v>63</v>
       </c>
       <c r="F113" t="s">
-        <v>16</v>
-      </c>
-      <c r="G113" t="s">
-        <v>17</v>
+        <v>60</v>
+      </c>
+      <c r="G113">
+        <v>0</v>
       </c>
       <c r="H113">
         <v>0</v>
       </c>
-      <c r="I113" t="s">
-        <v>44</v>
+      <c r="I113">
+        <v>100</v>
       </c>
     </row>
     <row r="114" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A114" t="s">
-        <v>202</v>
+        <v>195</v>
       </c>
       <c r="B114" t="s">
-        <v>45</v>
+        <v>12</v>
       </c>
       <c r="C114" t="s">
-        <v>46</v>
+        <v>13</v>
       </c>
       <c r="D114" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="E114" t="s">
-        <v>43</v>
+        <v>15</v>
       </c>
       <c r="F114" t="s">
         <v>16</v>
@@ -4963,27 +4982,27 @@
         <v>17</v>
       </c>
       <c r="H114">
-        <v>0.1</v>
+        <v>0</v>
       </c>
       <c r="I114">
-        <v>20</v>
+        <v>3</v>
       </c>
     </row>
     <row r="115" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A115" t="s">
-        <v>202</v>
+        <v>195</v>
       </c>
       <c r="B115" t="s">
-        <v>47</v>
+        <v>18</v>
       </c>
       <c r="C115" t="s">
-        <v>48</v>
+        <v>19</v>
       </c>
       <c r="D115" t="s">
         <v>14</v>
       </c>
       <c r="E115" t="s">
-        <v>49</v>
+        <v>15</v>
       </c>
       <c r="F115" t="s">
         <v>16</v>
@@ -4995,24 +5014,24 @@
         <v>0</v>
       </c>
       <c r="I115">
-        <v>100</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="116" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A116" t="s">
-        <v>202</v>
+        <v>195</v>
       </c>
       <c r="B116" t="s">
-        <v>165</v>
+        <v>20</v>
       </c>
       <c r="C116" t="s">
-        <v>166</v>
+        <v>21</v>
       </c>
       <c r="D116" t="s">
-        <v>14</v>
+        <v>200</v>
       </c>
       <c r="E116" t="s">
-        <v>70</v>
+        <v>15</v>
       </c>
       <c r="F116" t="s">
         <v>16</v>
@@ -5020,34 +5039,34 @@
       <c r="G116" t="s">
         <v>17</v>
       </c>
-      <c r="H116">
-        <v>0</v>
+      <c r="H116" s="1">
+        <v>9.9999999999999995E-7</v>
       </c>
       <c r="I116">
-        <v>100</v>
+        <v>10</v>
       </c>
     </row>
     <row r="117" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A117" t="s">
-        <v>202</v>
+        <v>195</v>
       </c>
       <c r="B117" t="s">
-        <v>203</v>
+        <v>22</v>
       </c>
       <c r="C117" t="s">
-        <v>204</v>
+        <v>23</v>
       </c>
       <c r="D117" t="s">
-        <v>93</v>
+        <v>24</v>
       </c>
       <c r="E117" t="s">
-        <v>43</v>
+        <v>15</v>
       </c>
       <c r="F117" t="s">
         <v>16</v>
       </c>
-      <c r="G117">
-        <v>0</v>
+      <c r="G117" t="s">
+        <v>17</v>
       </c>
       <c r="H117">
         <v>0</v>
@@ -5058,28 +5077,28 @@
     </row>
     <row r="118" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A118" t="s">
+        <v>195</v>
+      </c>
+      <c r="B118" t="s">
+        <v>25</v>
+      </c>
+      <c r="C118" t="s">
+        <v>26</v>
+      </c>
+      <c r="D118" t="s">
         <v>202</v>
       </c>
-      <c r="B118" t="s">
-        <v>171</v>
-      </c>
-      <c r="C118" t="s">
-        <v>172</v>
-      </c>
-      <c r="D118" t="s">
-        <v>93</v>
-      </c>
       <c r="E118" t="s">
-        <v>70</v>
+        <v>15</v>
       </c>
       <c r="F118" t="s">
         <v>16</v>
       </c>
-      <c r="G118">
-        <v>0</v>
-      </c>
-      <c r="H118">
-        <v>0</v>
+      <c r="G118" t="s">
+        <v>17</v>
+      </c>
+      <c r="H118" s="1">
+        <v>9.9999999999999995E-7</v>
       </c>
       <c r="I118">
         <v>1</v>
@@ -5087,19 +5106,19 @@
     </row>
     <row r="119" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A119" t="s">
+        <v>195</v>
+      </c>
+      <c r="B119" t="s">
+        <v>27</v>
+      </c>
+      <c r="C119" t="s">
+        <v>28</v>
+      </c>
+      <c r="D119" t="s">
         <v>202</v>
       </c>
-      <c r="B119" t="s">
-        <v>50</v>
-      </c>
-      <c r="C119" t="s">
-        <v>51</v>
-      </c>
-      <c r="D119" t="s">
-        <v>228</v>
-      </c>
       <c r="E119" t="s">
-        <v>52</v>
+        <v>15</v>
       </c>
       <c r="F119" t="s">
         <v>16</v>
@@ -5107,28 +5126,28 @@
       <c r="G119" t="s">
         <v>17</v>
       </c>
-      <c r="H119">
-        <v>0</v>
-      </c>
-      <c r="I119" t="s">
-        <v>44</v>
+      <c r="H119" s="1">
+        <v>1E-4</v>
+      </c>
+      <c r="I119">
+        <v>1</v>
       </c>
     </row>
     <row r="120" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A120" t="s">
-        <v>202</v>
+        <v>195</v>
       </c>
       <c r="B120" t="s">
-        <v>53</v>
+        <v>33</v>
       </c>
       <c r="C120" t="s">
-        <v>54</v>
+        <v>34</v>
       </c>
       <c r="D120" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="E120" t="s">
-        <v>52</v>
+        <v>15</v>
       </c>
       <c r="F120" t="s">
         <v>16</v>
@@ -5137,27 +5156,27 @@
         <v>17</v>
       </c>
       <c r="H120">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="I120">
-        <v>10</v>
+        <v>40</v>
       </c>
     </row>
     <row r="121" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A121" t="s">
-        <v>202</v>
+        <v>195</v>
       </c>
       <c r="B121" t="s">
-        <v>55</v>
+        <v>35</v>
       </c>
       <c r="C121" t="s">
-        <v>56</v>
+        <v>36</v>
       </c>
       <c r="D121" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="E121" t="s">
-        <v>52</v>
+        <v>15</v>
       </c>
       <c r="F121" t="s">
         <v>16</v>
@@ -5169,36 +5188,384 @@
         <v>0</v>
       </c>
       <c r="I121">
-        <v>50</v>
+        <v>20</v>
       </c>
     </row>
     <row r="122" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A122" t="s">
-        <v>202</v>
+        <v>195</v>
       </c>
       <c r="B122" t="s">
-        <v>162</v>
+        <v>37</v>
       </c>
       <c r="C122" t="s">
+        <v>38</v>
+      </c>
+      <c r="D122" t="s">
+        <v>204</v>
+      </c>
+      <c r="E122" t="s">
+        <v>15</v>
+      </c>
+      <c r="F122" t="s">
+        <v>16</v>
+      </c>
+      <c r="G122" t="s">
+        <v>17</v>
+      </c>
+      <c r="H122">
+        <v>10</v>
+      </c>
+      <c r="I122">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="123" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A123" t="s">
+        <v>195</v>
+      </c>
+      <c r="B123" t="s">
+        <v>39</v>
+      </c>
+      <c r="C123" t="s">
+        <v>40</v>
+      </c>
+      <c r="D123" t="s">
+        <v>205</v>
+      </c>
+      <c r="E123" t="s">
+        <v>15</v>
+      </c>
+      <c r="F123" t="s">
+        <v>16</v>
+      </c>
+      <c r="G123" t="s">
+        <v>17</v>
+      </c>
+      <c r="H123">
+        <v>20</v>
+      </c>
+      <c r="I123">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="124" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A124" t="s">
+        <v>195</v>
+      </c>
+      <c r="B124" t="s">
+        <v>41</v>
+      </c>
+      <c r="C124" t="s">
+        <v>42</v>
+      </c>
+      <c r="D124" t="s">
         <v>206</v>
       </c>
-      <c r="D122" t="s">
-        <v>217</v>
-      </c>
-      <c r="E122" t="s">
+      <c r="E124" t="s">
+        <v>43</v>
+      </c>
+      <c r="F124" t="s">
+        <v>16</v>
+      </c>
+      <c r="G124" t="s">
+        <v>17</v>
+      </c>
+      <c r="H124">
+        <v>0</v>
+      </c>
+      <c r="I124" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="125" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A125" t="s">
+        <v>195</v>
+      </c>
+      <c r="B125" t="s">
+        <v>45</v>
+      </c>
+      <c r="C125" t="s">
+        <v>46</v>
+      </c>
+      <c r="D125" t="s">
+        <v>17</v>
+      </c>
+      <c r="E125" t="s">
+        <v>43</v>
+      </c>
+      <c r="F125" t="s">
+        <v>16</v>
+      </c>
+      <c r="G125" t="s">
+        <v>17</v>
+      </c>
+      <c r="H125">
+        <v>0.1</v>
+      </c>
+      <c r="I125">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="126" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A126" t="s">
+        <v>195</v>
+      </c>
+      <c r="B126" t="s">
+        <v>158</v>
+      </c>
+      <c r="C126" t="s">
+        <v>159</v>
+      </c>
+      <c r="D126" t="s">
+        <v>14</v>
+      </c>
+      <c r="E126" t="s">
+        <v>63</v>
+      </c>
+      <c r="F126" t="s">
+        <v>16</v>
+      </c>
+      <c r="G126" t="s">
+        <v>17</v>
+      </c>
+      <c r="H126">
+        <v>0</v>
+      </c>
+      <c r="I126">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="127" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A127" t="s">
+        <v>195</v>
+      </c>
+      <c r="B127" t="s">
+        <v>196</v>
+      </c>
+      <c r="C127" t="s">
+        <v>197</v>
+      </c>
+      <c r="D127" t="s">
+        <v>86</v>
+      </c>
+      <c r="E127" t="s">
+        <v>43</v>
+      </c>
+      <c r="F127" t="s">
+        <v>16</v>
+      </c>
+      <c r="G127">
+        <v>0</v>
+      </c>
+      <c r="H127">
+        <v>0</v>
+      </c>
+      <c r="I127">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="128" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A128" t="s">
+        <v>195</v>
+      </c>
+      <c r="B128" t="s">
+        <v>164</v>
+      </c>
+      <c r="C128" t="s">
+        <v>165</v>
+      </c>
+      <c r="D128" t="s">
+        <v>86</v>
+      </c>
+      <c r="E128" t="s">
+        <v>63</v>
+      </c>
+      <c r="F128" t="s">
+        <v>16</v>
+      </c>
+      <c r="G128">
+        <v>0</v>
+      </c>
+      <c r="H128">
+        <v>0</v>
+      </c>
+      <c r="I128">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="129" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A129" t="s">
+        <v>195</v>
+      </c>
+      <c r="B129" t="s">
+        <v>47</v>
+      </c>
+      <c r="C129" t="s">
+        <v>48</v>
+      </c>
+      <c r="D129" t="s">
+        <v>221</v>
+      </c>
+      <c r="E129" t="s">
+        <v>49</v>
+      </c>
+      <c r="F129" t="s">
+        <v>16</v>
+      </c>
+      <c r="G129" t="s">
+        <v>17</v>
+      </c>
+      <c r="H129">
+        <v>0</v>
+      </c>
+      <c r="I129" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="130" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A130" t="s">
+        <v>195</v>
+      </c>
+      <c r="B130" t="s">
+        <v>50</v>
+      </c>
+      <c r="C130" t="s">
+        <v>51</v>
+      </c>
+      <c r="D130" t="s">
+        <v>198</v>
+      </c>
+      <c r="E130" t="s">
+        <v>49</v>
+      </c>
+      <c r="F130" t="s">
+        <v>16</v>
+      </c>
+      <c r="G130" t="s">
+        <v>17</v>
+      </c>
+      <c r="H130">
+        <v>0</v>
+      </c>
+      <c r="I130">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="131" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A131" t="s">
+        <v>195</v>
+      </c>
+      <c r="B131" t="s">
         <v>52</v>
       </c>
-      <c r="F122" t="s">
-        <v>16</v>
-      </c>
-      <c r="G122">
-        <v>0</v>
-      </c>
-      <c r="H122">
-        <v>0</v>
-      </c>
-      <c r="I122" t="s">
+      <c r="C131" t="s">
+        <v>53</v>
+      </c>
+      <c r="D131" t="s">
+        <v>198</v>
+      </c>
+      <c r="E131" t="s">
+        <v>49</v>
+      </c>
+      <c r="F131" t="s">
+        <v>16</v>
+      </c>
+      <c r="G131" t="s">
+        <v>17</v>
+      </c>
+      <c r="H131">
+        <v>0</v>
+      </c>
+      <c r="I131">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="132" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A132" t="s">
+        <v>195</v>
+      </c>
+      <c r="B132" t="s">
+        <v>155</v>
+      </c>
+      <c r="C132" t="s">
+        <v>199</v>
+      </c>
+      <c r="D132" t="s">
+        <v>210</v>
+      </c>
+      <c r="E132" t="s">
+        <v>49</v>
+      </c>
+      <c r="F132" t="s">
+        <v>16</v>
+      </c>
+      <c r="G132">
+        <v>0</v>
+      </c>
+      <c r="H132">
+        <v>0</v>
+      </c>
+      <c r="I132" t="s">
         <v>44</v>
+      </c>
+    </row>
+    <row r="133" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A133" t="s">
+        <v>195</v>
+      </c>
+      <c r="B133" t="s">
+        <v>29</v>
+      </c>
+      <c r="C133" t="s">
+        <v>30</v>
+      </c>
+      <c r="D133" t="s">
+        <v>24</v>
+      </c>
+      <c r="E133" t="s">
+        <v>15</v>
+      </c>
+      <c r="F133" t="s">
+        <v>16</v>
+      </c>
+      <c r="G133" t="s">
+        <v>17</v>
+      </c>
+      <c r="H133">
+        <v>0</v>
+      </c>
+      <c r="I133" s="1">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="134" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A134" t="s">
+        <v>195</v>
+      </c>
+      <c r="B134" t="s">
+        <v>31</v>
+      </c>
+      <c r="C134" t="s">
+        <v>32</v>
+      </c>
+      <c r="D134" t="s">
+        <v>14</v>
+      </c>
+      <c r="E134" t="s">
+        <v>15</v>
+      </c>
+      <c r="F134" t="s">
+        <v>16</v>
+      </c>
+      <c r="G134" t="s">
+        <v>17</v>
+      </c>
+      <c r="H134">
+        <v>0</v>
+      </c>
+      <c r="I134">
+        <v>3</v>
       </c>
     </row>
   </sheetData>

</xml_diff>